<commit_message>
now in returned dataframe elements are not anonymous anymore
</commit_message>
<xml_diff>
--- a/group_assignments.xlsx
+++ b/group_assignments.xlsx
@@ -468,22 +468,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Yannis Asproudis</t>
+          <t>Maitreyee Bhalme</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ioannis.asproudis@astrazeneca.com</t>
+          <t>maitreyee.bhalme@astrazeneca.com</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
+          <t>Master's student</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>Bioscience</t>
         </is>
       </c>
     </row>
@@ -495,17 +495,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Elena Grobecker</t>
+          <t>Yannis Asproudis</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>elena.grobecker@astrazeneca.com</t>
+          <t>ioannis.asproudis@astrazeneca.com</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>PhD student</t>
+          <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -522,22 +522,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Charline Sommer</t>
+          <t>Ida Näslund</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Charline.sommer@astrazeneca.com</t>
+          <t>ida.naslund1@astrazeneca.com</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Post doc</t>
+          <t>Master's student</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>Data and AI</t>
         </is>
       </c>
     </row>
@@ -549,49 +549,49 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Yuan Wei</t>
+          <t>Susanne Sauer</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>yuan.wei7@astrazeneca.com</t>
+          <t>susanne.sauer@astrazeneca.com</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Master's student</t>
+          <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Data and AI</t>
+          <t>Chemistry</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Group-2</t>
+          <t>Group-1</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Anna von Sydow</t>
+          <t>Mona Tilly</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>anna.vonsydow@astrazeneca.com</t>
+          <t>mona.tilly@astrazeneca.com</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Graduate</t>
+          <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Data and AI</t>
+          <t>Pharmaceutical Science</t>
         </is>
       </c>
     </row>
@@ -603,22 +603,22 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Emma Källstig</t>
+          <t>Elena Grobecker</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>emma.kallstig@astrazeneca.com</t>
+          <t>elena.grobecker@astrazeneca.com</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
+          <t>PhD student</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>Pharmaceutical Science</t>
         </is>
       </c>
     </row>
@@ -630,22 +630,22 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Mia Melhuish</t>
+          <t>Yuan Wei</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>mia.melhuish1@astrazeneca.net</t>
+          <t>yuan.wei7@astrazeneca.com</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Graduate</t>
+          <t>Master's student</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>Data and AI</t>
         </is>
       </c>
     </row>
@@ -657,76 +657,76 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Víctor López Juan</t>
+          <t>Linn Hellberg</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>victor.lopezjuan@astrazeneca.com</t>
+          <t>linn.hellberg1@astrazeneca.com</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
+          <t>Master's student</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Clinical trials</t>
+          <t>Data and AI</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Group-3</t>
+          <t>Group-2</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Christina Chau</t>
+          <t xml:space="preserve">Yousra Yahia </t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>christina.chau@astrazeneca.com</t>
+          <t>Yousra.yahia@astrazeneca.com</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
+          <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>Bioscience</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Group-3</t>
+          <t>Group-2</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Michalis</t>
+          <t>Sushanthika gnanasekaran</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>michail.fardis@astrazeneca.com</t>
+          <t>sushanthika.gnanasekaran@astrazeneca.com</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
+          <t>Master's student</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Clinical trials</t>
+          <t>Data and AI</t>
         </is>
       </c>
     </row>
@@ -738,17 +738,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Elisa Lai</t>
+          <t>Özge Yoluk</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>yonglin.lai@astrazeneca.com</t>
+          <t>ozge.yoluk@astrazeneca.com</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>PhD student</t>
+          <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -765,12 +765,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Fabricio Belgrano</t>
+          <t xml:space="preserve">Elin Benatti </t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>fabricio.belgrano@astrazeneca.com</t>
+          <t>elin.benatti1@astrazeneca.com</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -780,24 +780,24 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Intellectual Property</t>
+          <t>Bioscience</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Group-4</t>
+          <t>Group-3</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Evgeniia Berishvili</t>
+          <t>Pavlos Kashioulis</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>evgeniia.berishvili@astrazeneca.com</t>
+          <t>pavlos.kashioulis@astrazeneca.com</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -807,51 +807,51 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Regulatory</t>
+          <t>Clinical trials</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Group-4</t>
+          <t>Group-3</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Mona Tilly</t>
+          <t>Laura van Weesep</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>mona.tilly@astrazeneca.com</t>
+          <t>lauradesire.vanweesep@astrazeneca.com</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
+          <t>PhD student</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>Data and AI</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Group-4</t>
+          <t>Group-3</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Gabriel Abreu</t>
+          <t>Barbara Adamczyk</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>gabriel.abreu@astrazeneca.com</t>
+          <t>barbara.adamczyk@astrazeneca.com</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -861,7 +861,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Clinical trials</t>
+          <t>Pharmaceutical Science</t>
         </is>
       </c>
     </row>
@@ -873,12 +873,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Yinan Song</t>
+          <t>Maëlys Chastel</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Yinan.song@astrazeneca.com</t>
+          <t>maelys.chastel@astrazeneca.com</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -888,29 +888,29 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>DS AssayDev</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Group-5</t>
+          <t>Group-4</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Oliver Ekfeldt Hedberg</t>
+          <t>Víctor López Juan</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>oliver.ekfeldthedberg@hotmail.com</t>
+          <t>victor.lopezjuan@astrazeneca.com</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Master's student</t>
+          <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -922,17 +922,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Group-5</t>
+          <t>Group-4</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Miriam Cipullo</t>
+          <t>Charline Sommer</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>miriam.cipullo@astrazeneca.com</t>
+          <t>Charline.sommer@astrazeneca.com</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -949,17 +949,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Group-5</t>
+          <t>Group-4</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Alina Khramova</t>
+          <t>Alma söderström</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Alina.khramova@astrazeneca.com</t>
+          <t>Alma.soderstrom@astrazeneca.com</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -969,78 +969,78 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Management</t>
+          <t>Clinical trials</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Group-5</t>
+          <t>Group-4</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Yogesh Aher</t>
+          <t>Virginia Ramos</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>yogesh.aher@astrazeneca.com</t>
+          <t xml:space="preserve">virginia.ramos@astrazeneca.com    </t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
+          <t>Master's student</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Science generic</t>
+          <t>DMPK</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Group-6</t>
+          <t>Group-5</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Philip Dalsbecker</t>
+          <t>Umul-Khair Noor</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>philip.dalsbecker@astrazeneca.com</t>
+          <t>umul-khair.noor@astrazeneca.com</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Post doc</t>
+          <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>Regulatory</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Group-6</t>
+          <t>Group-5</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Gerard Masdeu</t>
+          <t>Bhavik Chouhan</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>gerard.masdeu@astrazeneca.com</t>
+          <t>bhavik.chouhan@astrazeneca.com</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1050,56 +1050,56 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>Data and AI</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Group-6</t>
+          <t>Group-5</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Manu Kanti</t>
+          <t>Megan Lee</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>manumanjunath.kanti@astrazeneca.com</t>
+          <t>megan.lee2@astrazeneca.com</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
+          <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>Innovation</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Group-6</t>
+          <t>Group-5</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Laura van Weesep</t>
+          <t>Anna von Sydow</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>lauradesire.vanweesep@astrazeneca.com</t>
+          <t>anna.vonsydow@astrazeneca.com</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>PhD student</t>
+          <t>Graduate</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1111,71 +1111,71 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Group-7</t>
+          <t>Group-5</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Lars Löfgren</t>
+          <t>Holly Longhurst</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Lars.lofgren@astrazeneca.com</t>
+          <t>holly.longhurst@astrazeneca.com</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Senior position (&gt;10 years experience)</t>
+          <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Translational Science &amp; Experimental Medicine</t>
+          <t>Pharmaceutical Science</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Group-7</t>
+          <t>Group-6</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Naixuan Liao</t>
+          <t>Giulia Botta</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>naixuan.liao@astrazeneca.com</t>
+          <t>giulia.botta@astrazeneca.com</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
+          <t>Graduate</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>Chemistry</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Group-7</t>
+          <t>Group-6</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Danielle Paterson</t>
+          <t>Manu Kanti</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>danielle.paterson@astrazeneca.com</t>
+          <t>manumanjunath.kanti@astrazeneca.com</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1185,29 +1185,29 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>Bioscience</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Group-7</t>
+          <t>Group-6</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Hannes Johansson</t>
+          <t>Amir Tohidi</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>hannes.johansson@astrazeneca.com</t>
+          <t>amir.tohidi@astrazeneca.com</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Graduate</t>
+          <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1219,71 +1219,71 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Group-8</t>
+          <t>Group-6</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Jessica Eriksson</t>
+          <t>Ulrike Ulbricht</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>jessica.eriksson1@astrazeneca.com</t>
+          <t>Ulrike.ulbricht@astrazeneca.com</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
+          <t>Senior position (&gt;10 years experience)</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>Clinical trials</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Group-8</t>
+          <t>Group-6</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Hemapriya Kothuru Chinnadurai</t>
+          <t>Cristina Secianski</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>hemapriyakothuru.chinnadurai@astrazeneca.com</t>
+          <t>cristina.secianski@astrazeneca.com</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Master's student</t>
+          <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>Regulatory</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Group-8</t>
+          <t>Group-7</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Aikaterini Emmanouilidi</t>
+          <t>Salma Nahra</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>aikaterini.emmanouilidi@astrazeneca.com</t>
+          <t>salma.nahra1@astrazeneca.com</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1293,24 +1293,24 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Clinical trials</t>
+          <t>Pharmaceutical Science</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Group-8</t>
+          <t>Group-7</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Purusothaman Seenivasan</t>
+          <t>Oliver Ekfeldt Hedberg</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>purusothaman.seenivasan@astrazeneca.com</t>
+          <t>oliver.ekfeldthedberg@hotmail.com</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1320,29 +1320,29 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Data and AI</t>
+          <t>Clinical trials</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Group-9</t>
+          <t>Group-7</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Fatima Eken</t>
+          <t>Sophie You</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Kdht135@astrazeneca.com</t>
+          <t>sophie.you@astrazeneca.com</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
+          <t>Master's student</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1354,7 +1354,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Group-9</t>
+          <t>Group-7</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1381,17 +1381,17 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Group-9</t>
+          <t>Group-7</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Aditya Soni</t>
+          <t>Danielle Paterson</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>aditya.soni@astrazeneca.com</t>
+          <t>danielle.paterson@astrazeneca.com</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1401,230 +1401,230 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Discovery Sciences</t>
+          <t>Chemistry</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Group-9</t>
+          <t>Group-8</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Adia Groza</t>
+          <t>Andrea Elser</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>adia.groza@astrazeneca.com</t>
+          <t>andrea.elser@astrazeneca.com</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Senior position (&gt;10 years experience)</t>
+          <t>Post doc</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Quality</t>
+          <t>Bioscience</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Group-10</t>
+          <t>Group-8</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Alma söderström</t>
+          <t>Johan Almlöf Ljungberg</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Alma.soderstrom@astrazeneca.com</t>
+          <t>johan.almlofljungberg1@astrazeneca.com</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
+          <t>Graduate</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Clinical trials</t>
+          <t>Pharmaceutical Science</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Group-10</t>
+          <t>Group-8</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Sushanthika gnanasekaran</t>
+          <t>Naixuan Liao</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>sushanthika.gnanasekaran@astrazeneca.com</t>
+          <t>naixuan.liao@astrazeneca.com</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Master's student</t>
+          <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Data and AI</t>
+          <t>Bioscience</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Group-10</t>
+          <t>Group-8</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Sophie You</t>
+          <t>Nina Koo</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>sophie.you@astrazeneca.com</t>
+          <t>hyewonnina.koo@astrazeneca.com</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Master's student</t>
+          <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>Data and AI</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Group-10</t>
+          <t>Group-8</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t xml:space="preserve">Johanna Holm </t>
+          <t>Kim Stockfelt</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Johanna.holm@astrazeneca.com</t>
+          <t>Kim.stockfelt@astrazeneca.com</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
+          <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Quality</t>
+          <t>Pharmaceutical Science</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Group-11</t>
+          <t>Group-9</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Amir Tohidi</t>
+          <t>Elisa Lai</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>amir.tohidi@astrazeneca.com</t>
+          <t>yonglin.lai@astrazeneca.com</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
+          <t>PhD student</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Information Technology</t>
+          <t>Chemistry</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Group-11</t>
+          <t>Group-9</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Melanie Hendrix</t>
+          <t>Gabriel Abreu</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>melanie.hendrix@astrazeneca.com</t>
+          <t>gabriel.abreu@astrazeneca.com</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
+          <t>Senior position (&gt;10 years experience)</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Regulatory</t>
+          <t>Clinical trials</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Group-11</t>
+          <t>Group-9</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t xml:space="preserve">Jennifer Sjulander </t>
+          <t>Arthur Herren</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Jennifer.sjulander2@astrazeneca.com</t>
+          <t>Arthur.herren@astrazeneca.com</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
+          <t>Master's student</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Sustainability in R&amp;D</t>
+          <t>Pharmaceutical Science</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Group-11</t>
+          <t>Group-9</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1651,152 +1651,152 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Group-12</t>
+          <t>Group-9</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Lakshidaa</t>
+          <t>Charlotte Galipaud</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>lakshidaa.saigiridharan@astrazeneca.com</t>
+          <t>charlotte.galipaud@astrazeneca.com</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
+          <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Data and AI</t>
+          <t>Bioscience</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Group-12</t>
+          <t>Group-10</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Manesh Nautiyal</t>
+          <t>Hemapriya Kothuru Chinnadurai</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Manesh.nautiyal@astrazeneca.com</t>
+          <t>hemapriyakothuru.chinnadurai@astrazeneca.com</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
+          <t>Master's student</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>Bioscience</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Group-12</t>
+          <t>Group-10</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Tho Nguyen</t>
+          <t>Madeleine Jolliffe</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>tho.nguyen1@astrazeneca.com</t>
+          <t>maddi.jolliffe@astrazenca.com</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
+          <t>Graduate</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>Bioscience</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Group-12</t>
+          <t>Group-10</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Pavlos Kashioulis</t>
+          <t>Maher abduljabbar</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>pavlos.kashioulis@astrazeneca.com</t>
+          <t>maher.abduljabbaral-barooki@astrazeneca.com</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
+          <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Clinical trials</t>
+          <t>Pharmaceutical Science</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Group-13</t>
+          <t>Group-10</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Maitreyee Bhalme</t>
+          <t xml:space="preserve">Jennifer Sjulander </t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>maitreyee.bhalme@astrazeneca.com</t>
+          <t>Jennifer.sjulander2@astrazeneca.com</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Master's student</t>
+          <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>Sustainability in R&amp;D</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Group-13</t>
+          <t>Group-10</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Pernilla Rumin</t>
+          <t>Evgeniia Berishvili</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>pernilla.rumin@astrazeneca.com</t>
+          <t>evgeniia.berishvili@astrazeneca.com</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1806,105 +1806,105 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Clinical trials</t>
+          <t>Regulatory</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Group-13</t>
+          <t>Group-11</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Camille Riff</t>
+          <t>Christina Chau</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Camille.riff@astrazeneca.com</t>
+          <t>christina.chau@astrazeneca.com</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
+          <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t xml:space="preserve">CPQP </t>
+          <t>Pharmaceutical Science</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Group-13</t>
+          <t>Group-11</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Umul-Khair Noor</t>
+          <t>Lars Löfgren</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>umul-khair.noor@astrazeneca.com</t>
+          <t>Lars.lofgren@astrazeneca.com</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
+          <t>Senior position (&gt;10 years experience)</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Regulatory</t>
+          <t>Translational Science &amp; Experimental Medicine</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Group-14</t>
+          <t>Group-11</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Barbara Adamczyk</t>
+          <t>Philip Dalsbecker</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>barbara.adamczyk@astrazeneca.com</t>
+          <t>philip.dalsbecker@astrazeneca.com</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Senior position (&gt;10 years experience)</t>
+          <t>Post doc</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>Bioscience</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Group-14</t>
+          <t>Group-11</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Charlotte Galipaud</t>
+          <t>Alison Howett</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>charlotte.galipaud@astrazeneca.com</t>
+          <t>alison.howett@astrazeneca.com</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1914,267 +1914,267 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>Regulatory</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Group-14</t>
+          <t>Group-11</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Alison Howett</t>
+          <t>Purusothaman Seenivasan</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>alison.howett@astrazeneca.com</t>
+          <t>purusothaman.seenivasan@astrazeneca.com</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
+          <t>Master's student</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Regulatory</t>
+          <t>Data and AI</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Group-14</t>
+          <t>Group-12</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Madeleine Jolliffe</t>
+          <t>Aikaterini Emmanouilidi</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>maddi.jolliffe@astrazenca.com</t>
+          <t>aikaterini.emmanouilidi@astrazeneca.com</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Graduate</t>
+          <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>Clinical trials</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Group-15</t>
+          <t>Group-12</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Elena</t>
+          <t>Michalis</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>eleni.lazaridi@astrazeneca.com</t>
+          <t>michail.fardis@astrazeneca.com</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
+          <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>Clinical trials</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Group-15</t>
+          <t>Group-12</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Susanna Abrahmsen Alami</t>
+          <t>Camille Riff</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Susanna.Abrahmsen-alami@astrazeneca.com</t>
+          <t>Camille.riff@astrazeneca.com</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Senior position (&gt;10 years experience)</t>
+          <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t xml:space="preserve">CPQP </t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Group-15</t>
+          <t>Group-12</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Giulia Botta</t>
+          <t>Anna</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>giulia.botta@astrazeneca.com</t>
+          <t>anna.shiriaeva@astrazeneca.com</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Graduate</t>
+          <t>Post doc</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>Bioscience</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Group-15</t>
+          <t>Group-12</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Linn Hellberg</t>
+          <t>Gerard Masdeu</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>linn.hellberg1@astrazeneca.com</t>
+          <t>gerard.masdeu@astrazeneca.com</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Master's student</t>
+          <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Data and AI</t>
+          <t>Pharmaceutical Science</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Group-16</t>
+          <t>Group-13</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Andrea Elser</t>
+          <t>Tho Nguyen</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>andrea.elser@astrazeneca.com</t>
+          <t>tho.nguyen1@astrazeneca.com</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Post doc</t>
+          <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>Pharmaceutical Science</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Group-16</t>
+          <t>Group-13</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Özge Yoluk</t>
+          <t>Adia Groza</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>ozge.yoluk@astrazeneca.com</t>
+          <t>adia.groza@astrazeneca.com</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
+          <t>Senior position (&gt;10 years experience)</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>Quality</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Group-16</t>
+          <t>Group-13</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Nina Koo</t>
+          <t>Mia Melhuish</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>hyewonnina.koo@astrazeneca.com</t>
+          <t>mia.melhuish1@astrazeneca.net</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
+          <t>Graduate</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Data and AI</t>
+          <t>Bioscience</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Group-16</t>
+          <t>Group-13</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Maëlys Chastel</t>
+          <t>Melanie Hendrix</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>maelys.chastel@astrazeneca.com</t>
+          <t>melanie.hendrix@astrazeneca.com</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2184,105 +2184,105 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>DS AssayDev</t>
+          <t>Regulatory</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Group-17</t>
+          <t>Group-13</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Ida Näslund</t>
+          <t>Emma Källstig</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>ida.naslund1@astrazeneca.com</t>
+          <t>emma.kallstig@astrazeneca.com</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Master's student</t>
+          <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Data and AI</t>
+          <t>Bioscience</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Group-17</t>
+          <t>Group-14</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Elena Camara</t>
+          <t>Fatima Eken</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>elena.camara@astrazeneca.com</t>
+          <t>Kdht135@astrazeneca.com</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Senior position (&gt;10 years experience)</t>
+          <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>Pharmaceutical Science</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Group-17</t>
+          <t>Group-14</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Michael Guerzoni</t>
+          <t>Jessica Eriksson</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>michael.guerzoni@astrazeneca.com</t>
+          <t>jessica.eriksson1@astrazeneca.com</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Post doc</t>
+          <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>Pharmaceutical Science</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Group-17</t>
+          <t>Group-14</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Maher abduljabbar</t>
+          <t>Manesh Nautiyal</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>maher.abduljabbaral-barooki@astrazeneca.com</t>
+          <t>Manesh.nautiyal@astrazeneca.com</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2292,159 +2292,159 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>Chemistry</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Group-18</t>
+          <t>Group-14</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Salma Nahra</t>
+          <t>Elena</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>salma.nahra1@astrazeneca.com</t>
+          <t>eleni.lazaridi@astrazeneca.com</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
+          <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>Chemistry</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Group-18</t>
+          <t>Group-14</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Bhavik Chouhan</t>
+          <t>Susanna Abrahmsen Alami</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>bhavik.chouhan@astrazeneca.com</t>
+          <t>Susanna.Abrahmsen-alami@astrazeneca.com</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
+          <t>Senior position (&gt;10 years experience)</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Data and AI</t>
+          <t>Pharmaceutical Science</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Group-18</t>
+          <t>Group-15</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Virginia Ramos</t>
+          <t>Yogesh Aher</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t xml:space="preserve">virginia.ramos@astrazeneca.com    </t>
+          <t>yogesh.aher@astrazeneca.com</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Master's student</t>
+          <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>DMPK</t>
+          <t>Science generic</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Group-18</t>
+          <t>Group-15</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Kim Stockfelt</t>
+          <t>Aditya Soni</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Kim.stockfelt@astrazeneca.com</t>
+          <t>aditya.soni@astrazeneca.com</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
+          <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>Discovery Sciences</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Group-19</t>
+          <t>Group-15</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Julia Lebrethon</t>
+          <t>Elena Camara</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>julia.lebrethon@astrazeneca.com</t>
+          <t>elena.camara@astrazeneca.com</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Master's student</t>
+          <t>Senior position (&gt;10 years experience)</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>Bioscience</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Group-19</t>
+          <t>Group-15</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Saja Hasan</t>
+          <t xml:space="preserve">Johanna Holm </t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>saja.hasan@astrazeneca.com</t>
+          <t>Johanna.holm@astrazeneca.com</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2461,17 +2461,17 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Group-19</t>
+          <t>Group-15</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Cristina Secianski</t>
+          <t>Yinan Song</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>cristina.secianski@astrazeneca.com</t>
+          <t>Yinan.song@astrazeneca.com</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2481,83 +2481,83 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Regulatory</t>
+          <t>Chemistry</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Group-19</t>
+          <t>Group-16</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Johan Almlöf Ljungberg</t>
+          <t>Lara Hastenreiter</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>johan.almlofljungberg1@astrazeneca.com</t>
+          <t>lara.hastenreiter@astrazeneca.com</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Graduate</t>
+          <t>Contractor</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Group-20</t>
+          <t>Group-16</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Ulrike Ulbricht</t>
+          <t>Saja Hasan</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Ulrike.ulbricht@astrazeneca.com</t>
+          <t>saja.hasan@astrazeneca.com</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Senior position (&gt;10 years experience)</t>
+          <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Clinical trials</t>
+          <t>Quality</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Group-20</t>
+          <t>Group-16</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Anna</t>
+          <t>Alisa Kirkin</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>anna.shiriaeva@astrazeneca.com</t>
+          <t>alisa.kirkin@astrazeneca.com</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Post doc</t>
+          <t>Master's student</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
@@ -2569,17 +2569,17 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Group-20</t>
+          <t>Group-16</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Holly Longhurst</t>
+          <t>Fabricio Belgrano</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>holly.longhurst@astrazeneca.com</t>
+          <t>fabricio.belgrano@astrazeneca.com</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -2589,24 +2589,24 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>Intellectual Property</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Group-20</t>
+          <t>Group-16</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t xml:space="preserve">Yousra Yahia </t>
+          <t>Alina Khramova</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Yousra.yahia@astrazeneca.com</t>
+          <t>Alina.khramova@astrazeneca.com</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -2616,95 +2616,95 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Group-21</t>
+          <t>Group-17</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Susanne Sauer</t>
+          <t>Lakshidaa</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>susanne.sauer@astrazeneca.com</t>
+          <t>lakshidaa.saigiridharan@astrazeneca.com</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
+          <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>Data and AI</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Group-21</t>
+          <t>Group-17</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Arthur Herren</t>
+          <t>Pernilla Rumin</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Arthur.herren@astrazeneca.com</t>
+          <t>pernilla.rumin@astrazeneca.com</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Master's student</t>
+          <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>Clinical trials</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Group-21</t>
+          <t>Group-17</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Lara Hastenreiter</t>
+          <t>Michael Guerzoni</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>lara.hastenreiter@astrazeneca.com</t>
+          <t>michael.guerzoni@astrazeneca.com</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Contractor</t>
+          <t>Post doc</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>Chemistry</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Group-21</t>
+          <t>Group-17</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2731,22 +2731,22 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Group-22</t>
+          <t>Group-17</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Alisa Kirkin</t>
+          <t>Miriam Cipullo</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>alisa.kirkin@astrazeneca.com</t>
+          <t>miriam.cipullo@astrazeneca.com</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Master's student</t>
+          <t>Post doc</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
@@ -2758,54 +2758,54 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Group-22</t>
+          <t>Group-18</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t xml:space="preserve">Elin Benatti </t>
+          <t>Hannes Johansson</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>elin.benatti1@astrazeneca.com</t>
+          <t>hannes.johansson@astrazeneca.com</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
+          <t>Graduate</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>Information Technology</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Group-22</t>
+          <t>Group-18</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Megan Lee</t>
+          <t>Julia Lebrethon</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>megan.lee2@astrazeneca.com</t>
+          <t>julia.lebrethon@astrazeneca.com</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
+          <t>Master's student</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Innovation</t>
+          <t>Pharmaceutical Science</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Using Optimized Group Diversity Logic Now to Assign the groups
</commit_message>
<xml_diff>
--- a/group_assignments.xlsx
+++ b/group_assignments.xlsx
@@ -468,22 +468,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Maitreyee Bhalme</t>
+          <t>Christina Chau</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>maitreyee.bhalme@astrazeneca.com</t>
+          <t>christina.chau@astrazeneca.com</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Master's student</t>
+          <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>Pharmaceutical Science</t>
         </is>
       </c>
     </row>
@@ -495,22 +495,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Yannis Asproudis</t>
+          <t>Laura van Weesep</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ioannis.asproudis@astrazeneca.com</t>
+          <t>lauradesire.vanweesep@astrazeneca.com</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
+          <t>PhD student</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>Data and AI</t>
         </is>
       </c>
     </row>
@@ -522,22 +522,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Ida Näslund</t>
+          <t>Ulrike Ulbricht</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ida.naslund1@astrazeneca.com</t>
+          <t>Ulrike.ulbricht@astrazeneca.com</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Master's student</t>
+          <t>Senior position (&gt;10 years experience)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Data and AI</t>
+          <t>Clinical trials</t>
         </is>
       </c>
     </row>
@@ -549,22 +549,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Susanne Sauer</t>
+          <t>Gerard Masdeu</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>susanne.sauer@astrazeneca.com</t>
+          <t>gerard.masdeu@astrazeneca.com</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
+          <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>Pharmaceutical Science</t>
         </is>
       </c>
     </row>
@@ -576,12 +576,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Mona Tilly</t>
+          <t>Fabricio Belgrano</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>mona.tilly@astrazeneca.com</t>
+          <t>fabricio.belgrano@astrazeneca.com</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -591,7 +591,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>Intellectual Property</t>
         </is>
       </c>
     </row>
@@ -603,22 +603,22 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Elena Grobecker</t>
+          <t>Oliver Ekfeldt Hedberg</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>elena.grobecker@astrazeneca.com</t>
+          <t>oliver.ekfeldthedberg@hotmail.com</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>PhD student</t>
+          <t>Master's student</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>Clinical trials</t>
         </is>
       </c>
     </row>
@@ -630,22 +630,22 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Yuan Wei</t>
+          <t>Gabriel Abreu</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>yuan.wei7@astrazeneca.com</t>
+          <t>gabriel.abreu@astrazeneca.com</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Master's student</t>
+          <t>Senior position (&gt;10 years experience)</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Data and AI</t>
+          <t>Clinical trials</t>
         </is>
       </c>
     </row>
@@ -657,22 +657,22 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Linn Hellberg</t>
+          <t>Hannes Johansson</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>linn.hellberg1@astrazeneca.com</t>
+          <t>hannes.johansson@astrazeneca.com</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Master's student</t>
+          <t>Graduate</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Data and AI</t>
+          <t>Information Technology</t>
         </is>
       </c>
     </row>
@@ -684,22 +684,22 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Yousra Yahia </t>
+          <t>Elisa Lai</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Yousra.yahia@astrazeneca.com</t>
+          <t>yonglin.lai@astrazeneca.com</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
+          <t>PhD student</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>Chemistry</t>
         </is>
       </c>
     </row>
@@ -711,12 +711,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Sushanthika gnanasekaran</t>
+          <t>Sophie You</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>sushanthika.gnanasekaran@astrazeneca.com</t>
+          <t>sophie.you@astrazeneca.com</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -726,7 +726,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Data and AI</t>
+          <t>Pharmaceutical Science</t>
         </is>
       </c>
     </row>
@@ -738,22 +738,22 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Özge Yoluk</t>
+          <t>Virginia Ramos</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>ozge.yoluk@astrazeneca.com</t>
+          <t xml:space="preserve">virginia.ramos@astrazeneca.com    </t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
+          <t>Master's student</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>DMPK</t>
         </is>
       </c>
     </row>
@@ -765,22 +765,22 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Elin Benatti </t>
+          <t>Michalis</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>elin.benatti1@astrazeneca.com</t>
+          <t>michail.fardis@astrazeneca.com</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
+          <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>Clinical trials</t>
         </is>
       </c>
     </row>
@@ -792,12 +792,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Pavlos Kashioulis</t>
+          <t>Aikaterini Emmanouilidi</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>pavlos.kashioulis@astrazeneca.com</t>
+          <t>aikaterini.emmanouilidi@astrazeneca.com</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -819,22 +819,22 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Laura van Weesep</t>
+          <t>Mona Tilly</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>lauradesire.vanweesep@astrazeneca.com</t>
+          <t>mona.tilly@astrazeneca.com</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>PhD student</t>
+          <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Data and AI</t>
+          <t>Pharmaceutical Science</t>
         </is>
       </c>
     </row>
@@ -846,22 +846,22 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Barbara Adamczyk</t>
+          <t>Pernilla Rumin</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>barbara.adamczyk@astrazeneca.com</t>
+          <t>pernilla.rumin@astrazeneca.com</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Senior position (&gt;10 years experience)</t>
+          <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>Clinical trials</t>
         </is>
       </c>
     </row>
@@ -873,22 +873,22 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Maëlys Chastel</t>
+          <t>Madeleine Jolliffe</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>maelys.chastel@astrazeneca.com</t>
+          <t>maddi.jolliffe@astrazenca.com</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
+          <t>Graduate</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>DS AssayDev</t>
+          <t>Bioscience</t>
         </is>
       </c>
     </row>
@@ -900,22 +900,22 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Víctor López Juan</t>
+          <t>Evgeniia Berishvili</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>victor.lopezjuan@astrazeneca.com</t>
+          <t>evgeniia.berishvili@astrazeneca.com</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
+          <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Clinical trials</t>
+          <t>Regulatory</t>
         </is>
       </c>
     </row>
@@ -927,12 +927,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Charline Sommer</t>
+          <t>Philip Dalsbecker</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Charline.sommer@astrazeneca.com</t>
+          <t>philip.dalsbecker@astrazeneca.com</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -954,12 +954,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Alma söderström</t>
+          <t>Camille Riff</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Alma.soderstrom@astrazeneca.com</t>
+          <t>Camille.riff@astrazeneca.com</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -969,7 +969,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Clinical trials</t>
+          <t xml:space="preserve">CPQP </t>
         </is>
       </c>
     </row>
@@ -981,22 +981,22 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Virginia Ramos</t>
+          <t>Elena</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t xml:space="preserve">virginia.ramos@astrazeneca.com    </t>
+          <t>eleni.lazaridi@astrazeneca.com</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Master's student</t>
+          <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>DMPK</t>
+          <t>Chemistry</t>
         </is>
       </c>
     </row>
@@ -1008,22 +1008,22 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Umul-Khair Noor</t>
+          <t>Susanne Sauer</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>umul-khair.noor@astrazeneca.com</t>
+          <t>susanne.sauer@astrazeneca.com</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
+          <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Regulatory</t>
+          <t>Chemistry</t>
         </is>
       </c>
     </row>
@@ -1035,22 +1035,22 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Bhavik Chouhan</t>
+          <t>Arthur Herren</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>bhavik.chouhan@astrazeneca.com</t>
+          <t>Arthur.herren@astrazeneca.com</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
+          <t>Master's student</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Data and AI</t>
+          <t>Pharmaceutical Science</t>
         </is>
       </c>
     </row>
@@ -1062,12 +1062,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Megan Lee</t>
+          <t>Ingrid Lichtin</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>megan.lee2@astrazeneca.com</t>
+          <t>Ingrid.Lichtin@astrazeneca.com</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1077,7 +1077,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Innovation</t>
+          <t>Quality</t>
         </is>
       </c>
     </row>
@@ -1089,22 +1089,22 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Anna von Sydow</t>
+          <t>Fatima Eken</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>anna.vonsydow@astrazeneca.com</t>
+          <t>Kdht135@astrazeneca.com</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Graduate</t>
+          <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Data and AI</t>
+          <t>Pharmaceutical Science</t>
         </is>
       </c>
     </row>
@@ -1116,22 +1116,22 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Holly Longhurst</t>
+          <t>Andrea Elser</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>holly.longhurst@astrazeneca.com</t>
+          <t>andrea.elser@astrazeneca.com</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
+          <t>Post doc</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>Bioscience</t>
         </is>
       </c>
     </row>
@@ -1143,22 +1143,22 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Giulia Botta</t>
+          <t>Barbara Adamczyk</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>giulia.botta@astrazeneca.com</t>
+          <t>barbara.adamczyk@astrazeneca.com</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Graduate</t>
+          <t>Senior position (&gt;10 years experience)</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>Pharmaceutical Science</t>
         </is>
       </c>
     </row>
@@ -1170,22 +1170,22 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Manu Kanti</t>
+          <t>Salma Nahra</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>manumanjunath.kanti@astrazeneca.com</t>
+          <t>salma.nahra1@astrazeneca.com</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
+          <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>Pharmaceutical Science</t>
         </is>
       </c>
     </row>
@@ -1197,22 +1197,22 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Amir Tohidi</t>
+          <t>Anna von Sydow</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>amir.tohidi@astrazeneca.com</t>
+          <t>anna.vonsydow@astrazeneca.com</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
+          <t>Graduate</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Information Technology</t>
+          <t>Data and AI</t>
         </is>
       </c>
     </row>
@@ -1224,22 +1224,22 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Ulrike Ulbricht</t>
+          <t>Hemapriya Kothuru Chinnadurai</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Ulrike.ulbricht@astrazeneca.com</t>
+          <t>hemapriyakothuru.chinnadurai@astrazeneca.com</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Senior position (&gt;10 years experience)</t>
+          <t>Master's student</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Clinical trials</t>
+          <t>Bioscience</t>
         </is>
       </c>
     </row>
@@ -1251,12 +1251,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Cristina Secianski</t>
+          <t>Megan Lee</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>cristina.secianski@astrazeneca.com</t>
+          <t>megan.lee2@astrazeneca.com</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1266,7 +1266,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Regulatory</t>
+          <t>Innovation</t>
         </is>
       </c>
     </row>
@@ -1278,12 +1278,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Salma Nahra</t>
+          <t>Özge Yoluk</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>salma.nahra1@astrazeneca.com</t>
+          <t>ozge.yoluk@astrazeneca.com</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>Chemistry</t>
         </is>
       </c>
     </row>
@@ -1305,12 +1305,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Oliver Ekfeldt Hedberg</t>
+          <t>Maitreyee Bhalme</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>oliver.ekfeldthedberg@hotmail.com</t>
+          <t>maitreyee.bhalme@astrazeneca.com</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1320,7 +1320,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Clinical trials</t>
+          <t>Bioscience</t>
         </is>
       </c>
     </row>
@@ -1332,22 +1332,22 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Sophie You</t>
+          <t>Yogesh Aher</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>sophie.you@astrazeneca.com</t>
+          <t>yogesh.aher@astrazeneca.com</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Master's student</t>
+          <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>Science generic</t>
         </is>
       </c>
     </row>
@@ -1359,22 +1359,22 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Ingrid Lichtin</t>
+          <t>Maher abduljabbar</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Ingrid.Lichtin@astrazeneca.com</t>
+          <t>maher.abduljabbaral-barooki@astrazeneca.com</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
+          <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Quality</t>
+          <t>Pharmaceutical Science</t>
         </is>
       </c>
     </row>
@@ -1386,12 +1386,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Danielle Paterson</t>
+          <t>Emma Källstig</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>danielle.paterson@astrazeneca.com</t>
+          <t>emma.kallstig@astrazeneca.com</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1401,7 +1401,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>Bioscience</t>
         </is>
       </c>
     </row>
@@ -1413,22 +1413,22 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Andrea Elser</t>
+          <t>Ida Näslund</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>andrea.elser@astrazeneca.com</t>
+          <t>ida.naslund1@astrazeneca.com</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Post doc</t>
+          <t>Master's student</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>Data and AI</t>
         </is>
       </c>
     </row>
@@ -1440,22 +1440,22 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Johan Almlöf Ljungberg</t>
+          <t>Elena Camara</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>johan.almlofljungberg1@astrazeneca.com</t>
+          <t>elena.camara@astrazeneca.com</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Graduate</t>
+          <t>Senior position (&gt;10 years experience)</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>Bioscience</t>
         </is>
       </c>
     </row>
@@ -1467,12 +1467,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Naixuan Liao</t>
+          <t>Víctor López Juan</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>naixuan.liao@astrazeneca.com</t>
+          <t>victor.lopezjuan@astrazeneca.com</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1482,7 +1482,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>Clinical trials</t>
         </is>
       </c>
     </row>
@@ -1494,22 +1494,22 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Nina Koo</t>
+          <t xml:space="preserve">Johanna Holm </t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>hyewonnina.koo@astrazeneca.com</t>
+          <t>Johanna.holm@astrazeneca.com</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
+          <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Data and AI</t>
+          <t>Quality</t>
         </is>
       </c>
     </row>
@@ -1521,22 +1521,22 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Kim Stockfelt</t>
+          <t>Yuan Wei</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Kim.stockfelt@astrazeneca.com</t>
+          <t>yuan.wei7@astrazeneca.com</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
+          <t>Master's student</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>Data and AI</t>
         </is>
       </c>
     </row>
@@ -1548,22 +1548,22 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Elisa Lai</t>
+          <t>Sushanthika gnanasekaran</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>yonglin.lai@astrazeneca.com</t>
+          <t>sushanthika.gnanasekaran@astrazeneca.com</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>PhD student</t>
+          <t>Master's student</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>Data and AI</t>
         </is>
       </c>
     </row>
@@ -1575,22 +1575,22 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Gabriel Abreu</t>
+          <t>Yannis Asproudis</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>gabriel.abreu@astrazeneca.com</t>
+          <t>ioannis.asproudis@astrazeneca.com</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Senior position (&gt;10 years experience)</t>
+          <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Clinical trials</t>
+          <t>Pharmaceutical Science</t>
         </is>
       </c>
     </row>
@@ -1602,12 +1602,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Arthur Herren</t>
+          <t>Linn Hellberg</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Arthur.herren@astrazeneca.com</t>
+          <t>linn.hellberg1@astrazeneca.com</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1617,7 +1617,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>Data and AI</t>
         </is>
       </c>
     </row>
@@ -1629,22 +1629,22 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Nina Sandström</t>
+          <t>Mia Melhuish</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>nina.sandstrom@astrazeneca.com</t>
+          <t>mia.melhuish1@astrazeneca.net</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
+          <t>Graduate</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>FM</t>
+          <t>Bioscience</t>
         </is>
       </c>
     </row>
@@ -1656,12 +1656,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Charlotte Galipaud</t>
+          <t>Manesh Nautiyal</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>charlotte.galipaud@astrazeneca.com</t>
+          <t>Manesh.nautiyal@astrazeneca.com</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1671,7 +1671,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>Chemistry</t>
         </is>
       </c>
     </row>
@@ -1683,17 +1683,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Hemapriya Kothuru Chinnadurai</t>
+          <t>Anna</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>hemapriyakothuru.chinnadurai@astrazeneca.com</t>
+          <t>anna.shiriaeva@astrazeneca.com</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Master's student</t>
+          <t>Post doc</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -1710,22 +1710,22 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Madeleine Jolliffe</t>
+          <t>Adia Groza</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>maddi.jolliffe@astrazenca.com</t>
+          <t>adia.groza@astrazeneca.com</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Graduate</t>
+          <t>Senior position (&gt;10 years experience)</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>Quality</t>
         </is>
       </c>
     </row>
@@ -1737,17 +1737,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Maher abduljabbar</t>
+          <t>Jessica Eriksson</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>maher.abduljabbaral-barooki@astrazeneca.com</t>
+          <t>jessica.eriksson1@astrazeneca.com</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
+          <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -1764,22 +1764,22 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t xml:space="preserve">Jennifer Sjulander </t>
+          <t>Maëlys Chastel</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Jennifer.sjulander2@astrazeneca.com</t>
+          <t>maelys.chastel@astrazeneca.com</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
+          <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Sustainability in R&amp;D</t>
+          <t>DS AssayDev</t>
         </is>
       </c>
     </row>
@@ -1791,22 +1791,22 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Evgeniia Berishvili</t>
+          <t>Johan Almlöf Ljungberg</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>evgeniia.berishvili@astrazeneca.com</t>
+          <t>johan.almlofljungberg1@astrazeneca.com</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
+          <t>Graduate</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Regulatory</t>
+          <t>Pharmaceutical Science</t>
         </is>
       </c>
     </row>
@@ -1818,12 +1818,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Christina Chau</t>
+          <t>Naixuan Liao</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>christina.chau@astrazeneca.com</t>
+          <t>naixuan.liao@astrazeneca.com</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1833,7 +1833,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>Bioscience</t>
         </is>
       </c>
     </row>
@@ -1845,22 +1845,22 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Lars Löfgren</t>
+          <t>Julia Lebrethon</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Lars.lofgren@astrazeneca.com</t>
+          <t>julia.lebrethon@astrazeneca.com</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Senior position (&gt;10 years experience)</t>
+          <t>Master's student</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Translational Science &amp; Experimental Medicine</t>
+          <t>Pharmaceutical Science</t>
         </is>
       </c>
     </row>
@@ -1872,22 +1872,22 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Philip Dalsbecker</t>
+          <t>Alma söderström</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>philip.dalsbecker@astrazeneca.com</t>
+          <t>Alma.soderstrom@astrazeneca.com</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Post doc</t>
+          <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>Clinical trials</t>
         </is>
       </c>
     </row>
@@ -1899,22 +1899,22 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Alison Howett</t>
+          <t>Lara Hastenreiter</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>alison.howett@astrazeneca.com</t>
+          <t>lara.hastenreiter@astrazeneca.com</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
+          <t>Contractor</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Regulatory</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -1926,22 +1926,22 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Purusothaman Seenivasan</t>
+          <t>Elena Grobecker</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>purusothaman.seenivasan@astrazeneca.com</t>
+          <t>elena.grobecker@astrazeneca.com</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Master's student</t>
+          <t>PhD student</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Data and AI</t>
+          <t>Pharmaceutical Science</t>
         </is>
       </c>
     </row>
@@ -1953,22 +1953,22 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Aikaterini Emmanouilidi</t>
+          <t>Julia Ringwall</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>aikaterini.emmanouilidi@astrazeneca.com</t>
+          <t>julia.ringwall@astrazeneca.com</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
+          <t>Senior position (&gt;10 years experience)</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Clinical trials</t>
+          <t xml:space="preserve">Safety and Work environment </t>
         </is>
       </c>
     </row>
@@ -1980,22 +1980,22 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Michalis</t>
+          <t>Aditya Soni</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>michail.fardis@astrazeneca.com</t>
+          <t>aditya.soni@astrazeneca.com</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
+          <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Clinical trials</t>
+          <t>Discovery Sciences</t>
         </is>
       </c>
     </row>
@@ -2007,12 +2007,12 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Camille Riff</t>
+          <t>Cristina Secianski</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Camille.riff@astrazeneca.com</t>
+          <t>cristina.secianski@astrazeneca.com</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -2022,7 +2022,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t xml:space="preserve">CPQP </t>
+          <t>Regulatory</t>
         </is>
       </c>
     </row>
@@ -2034,17 +2034,17 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Anna</t>
+          <t>Charlotte Galipaud</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>anna.shiriaeva@astrazeneca.com</t>
+          <t>charlotte.galipaud@astrazeneca.com</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Post doc</t>
+          <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -2061,22 +2061,22 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Gerard Masdeu</t>
+          <t>Lars Löfgren</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>gerard.masdeu@astrazeneca.com</t>
+          <t>Lars.lofgren@astrazeneca.com</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
+          <t>Senior position (&gt;10 years experience)</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>Translational Science &amp; Experimental Medicine</t>
         </is>
       </c>
     </row>
@@ -2088,12 +2088,12 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Tho Nguyen</t>
+          <t>Amir Tohidi</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>tho.nguyen1@astrazeneca.com</t>
+          <t>amir.tohidi@astrazeneca.com</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -2103,7 +2103,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>Information Technology</t>
         </is>
       </c>
     </row>
@@ -2115,22 +2115,22 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Adia Groza</t>
+          <t>Alisa Kirkin</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>adia.groza@astrazeneca.com</t>
+          <t>alisa.kirkin@astrazeneca.com</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Senior position (&gt;10 years experience)</t>
+          <t>Master's student</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Quality</t>
+          <t>Bioscience</t>
         </is>
       </c>
     </row>
@@ -2142,22 +2142,22 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Mia Melhuish</t>
+          <t>Purusothaman Seenivasan</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>mia.melhuish1@astrazeneca.net</t>
+          <t>purusothaman.seenivasan@astrazeneca.com</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Graduate</t>
+          <t>Master's student</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>Data and AI</t>
         </is>
       </c>
     </row>
@@ -2169,12 +2169,12 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Melanie Hendrix</t>
+          <t>Umul-Khair Noor</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>melanie.hendrix@astrazeneca.com</t>
+          <t>umul-khair.noor@astrazeneca.com</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2196,22 +2196,22 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Emma Källstig</t>
+          <t>Nina Koo</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>emma.kallstig@astrazeneca.com</t>
+          <t>hyewonnina.koo@astrazeneca.com</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
+          <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>Data and AI</t>
         </is>
       </c>
     </row>
@@ -2223,12 +2223,12 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Fatima Eken</t>
+          <t>Saja Hasan</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Kdht135@astrazeneca.com</t>
+          <t>saja.hasan@astrazeneca.com</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2238,7 +2238,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>Quality</t>
         </is>
       </c>
     </row>
@@ -2250,22 +2250,22 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Jessica Eriksson</t>
+          <t>Giulia Botta</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>jessica.eriksson1@astrazeneca.com</t>
+          <t>giulia.botta@astrazeneca.com</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
+          <t>Graduate</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>Chemistry</t>
         </is>
       </c>
     </row>
@@ -2277,22 +2277,22 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Manesh Nautiyal</t>
+          <t>Melanie Hendrix</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Manesh.nautiyal@astrazeneca.com</t>
+          <t>melanie.hendrix@astrazeneca.com</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
+          <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>Regulatory</t>
         </is>
       </c>
     </row>
@@ -2304,12 +2304,12 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Elena</t>
+          <t>Danielle Paterson</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>eleni.lazaridi@astrazeneca.com</t>
+          <t>danielle.paterson@astrazeneca.com</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2331,22 +2331,22 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Susanna Abrahmsen Alami</t>
+          <t>Bhavik Chouhan</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Susanna.Abrahmsen-alami@astrazeneca.com</t>
+          <t>bhavik.chouhan@astrazeneca.com</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Senior position (&gt;10 years experience)</t>
+          <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>Data and AI</t>
         </is>
       </c>
     </row>
@@ -2358,12 +2358,12 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Yogesh Aher</t>
+          <t>Holly Longhurst</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>yogesh.aher@astrazeneca.com</t>
+          <t>holly.longhurst@astrazeneca.com</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -2373,7 +2373,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Science generic</t>
+          <t>Pharmaceutical Science</t>
         </is>
       </c>
     </row>
@@ -2385,22 +2385,22 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Aditya Soni</t>
+          <t>Susanna Abrahmsen Alami</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>aditya.soni@astrazeneca.com</t>
+          <t>Susanna.Abrahmsen-alami@astrazeneca.com</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
+          <t>Senior position (&gt;10 years experience)</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Discovery Sciences</t>
+          <t>Pharmaceutical Science</t>
         </is>
       </c>
     </row>
@@ -2412,22 +2412,22 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Elena Camara</t>
+          <t>Kim Stockfelt</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>elena.camara@astrazeneca.com</t>
+          <t>Kim.stockfelt@astrazeneca.com</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Senior position (&gt;10 years experience)</t>
+          <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>Pharmaceutical Science</t>
         </is>
       </c>
     </row>
@@ -2439,22 +2439,22 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t xml:space="preserve">Johanna Holm </t>
+          <t>Miriam Cipullo</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Johanna.holm@astrazeneca.com</t>
+          <t>miriam.cipullo@astrazeneca.com</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
+          <t>Post doc</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Quality</t>
+          <t>Bioscience</t>
         </is>
       </c>
     </row>
@@ -2466,22 +2466,22 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Yinan Song</t>
+          <t>Manu Kanti</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Yinan.song@astrazeneca.com</t>
+          <t>manumanjunath.kanti@astrazeneca.com</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
+          <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>Bioscience</t>
         </is>
       </c>
     </row>
@@ -2493,22 +2493,22 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Lara Hastenreiter</t>
+          <t>Yinan Song</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>lara.hastenreiter@astrazeneca.com</t>
+          <t>Yinan.song@astrazeneca.com</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Contractor</t>
+          <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>Chemistry</t>
         </is>
       </c>
     </row>
@@ -2520,22 +2520,22 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Saja Hasan</t>
+          <t>Lakshidaa</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>saja.hasan@astrazeneca.com</t>
+          <t>lakshidaa.saigiridharan@astrazeneca.com</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
+          <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Quality</t>
+          <t>Data and AI</t>
         </is>
       </c>
     </row>
@@ -2547,22 +2547,22 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Alisa Kirkin</t>
+          <t>Alina Khramova</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>alisa.kirkin@astrazeneca.com</t>
+          <t>Alina.khramova@astrazeneca.com</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Master's student</t>
+          <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
@@ -2574,22 +2574,22 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Fabricio Belgrano</t>
+          <t>Charline Sommer</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>fabricio.belgrano@astrazeneca.com</t>
+          <t>Charline.sommer@astrazeneca.com</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
+          <t>Post doc</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Intellectual Property</t>
+          <t>Bioscience</t>
         </is>
       </c>
     </row>
@@ -2601,22 +2601,22 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Alina Khramova</t>
+          <t xml:space="preserve">Elin Benatti </t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Alina.khramova@astrazeneca.com</t>
+          <t>elin.benatti1@astrazeneca.com</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
+          <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Management</t>
+          <t>Bioscience</t>
         </is>
       </c>
     </row>
@@ -2628,12 +2628,12 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Lakshidaa</t>
+          <t>Tho Nguyen</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>lakshidaa.saigiridharan@astrazeneca.com</t>
+          <t>tho.nguyen1@astrazeneca.com</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -2643,7 +2643,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Data and AI</t>
+          <t>Pharmaceutical Science</t>
         </is>
       </c>
     </row>
@@ -2655,12 +2655,12 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Pernilla Rumin</t>
+          <t>Pavlos Kashioulis</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>pernilla.rumin@astrazeneca.com</t>
+          <t>pavlos.kashioulis@astrazeneca.com</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -2682,22 +2682,22 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Michael Guerzoni</t>
+          <t>Alison Howett</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>michael.guerzoni@astrazeneca.com</t>
+          <t>alison.howett@astrazeneca.com</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Post doc</t>
+          <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>Regulatory</t>
         </is>
       </c>
     </row>
@@ -2709,22 +2709,22 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Julia Ringwall</t>
+          <t>Michael Guerzoni</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>julia.ringwall@astrazeneca.com</t>
+          <t>michael.guerzoni@astrazeneca.com</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Senior position (&gt;10 years experience)</t>
+          <t>Post doc</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t xml:space="preserve">Safety and Work environment </t>
+          <t>Chemistry</t>
         </is>
       </c>
     </row>
@@ -2736,22 +2736,22 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Miriam Cipullo</t>
+          <t xml:space="preserve">Jennifer Sjulander </t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>miriam.cipullo@astrazeneca.com</t>
+          <t>Jennifer.sjulander2@astrazeneca.com</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Post doc</t>
+          <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>Sustainability in R&amp;D</t>
         </is>
       </c>
     </row>
@@ -2763,22 +2763,22 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Hannes Johansson</t>
+          <t>Nina Sandström</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>hannes.johansson@astrazeneca.com</t>
+          <t>nina.sandstrom@astrazeneca.com</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Graduate</t>
+          <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Information Technology</t>
+          <t>FM</t>
         </is>
       </c>
     </row>
@@ -2790,22 +2790,22 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Julia Lebrethon</t>
+          <t xml:space="preserve">Yousra Yahia </t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>julia.lebrethon@astrazeneca.com</t>
+          <t>Yousra.yahia@astrazeneca.com</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Master's student</t>
+          <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>Bioscience</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed duplicate members and reassignment to same group
</commit_message>
<xml_diff>
--- a/group_assignments.xlsx
+++ b/group_assignments.xlsx
@@ -436,27 +436,27 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Group</t>
+          <t>Group ID</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Name2</t>
+          <t>Name</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Email (For AZ employees, use your.name@astrazeneca.com, but others are welcome too)</t>
+          <t>Position</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Which of the following best describes your position?</t>
+          <t>Sector</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Which of the following best describes your Job Family Group?</t>
+          <t>Email</t>
         </is>
       </c>
     </row>
@@ -468,22 +468,20 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Christina Chau</t>
+          <t>Oliver Ekfeldt Hedberg</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>christina.chau@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
-        </is>
+          <t>Master's student</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>oliver.ekfeldthedberg@hotmail.com</t>
         </is>
       </c>
     </row>
@@ -495,22 +493,20 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Laura van Weesep</t>
+          <t>Hannes Johansson</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>lauradesire.vanweesep@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>PhD student</t>
-        </is>
+          <t>Graduate</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>2</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Data and AI</t>
+          <t>hannes.johansson@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -522,22 +518,20 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Ulrike Ulbricht</t>
+          <t>Laura van Weesep</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Ulrike.ulbricht@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Senior position (&gt;10 years experience)</t>
-        </is>
+          <t>PhD student</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>3</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Clinical trials</t>
+          <t>lauradesire.vanweesep@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -554,17 +548,15 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>Mid-level position (3-10 years experience)</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>4</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>gerard.masdeu@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Mid-level position (3-10 years experience)</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Pharmaceutical Science</t>
         </is>
       </c>
     </row>
@@ -576,49 +568,45 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Fabricio Belgrano</t>
+          <t>Elisa Lai</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>fabricio.belgrano@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
-        </is>
+          <t>PhD student</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>5</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Intellectual Property</t>
+          <t>yonglin.lai@astrazeneca.com</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Group-2</t>
+          <t>Group-1</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Oliver Ekfeldt Hedberg</t>
+          <t>Ulrike Ulbricht</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>oliver.ekfeldthedberg@hotmail.com</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Master's student</t>
-        </is>
+          <t>Senior position (&gt;10 years experience)</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>86</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Clinical trials</t>
+          <t>Ulrike.ulbricht@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -630,22 +618,20 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Gabriel Abreu</t>
+          <t>Fabricio Belgrano</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>gabriel.abreu@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Senior position (&gt;10 years experience)</t>
-        </is>
+          <t>Entry-level position (&lt;3 years of experience)</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>6</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Clinical trials</t>
+          <t>fabricio.belgrano@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -657,22 +643,20 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Hannes Johansson</t>
+          <t>Virginia Ramos</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>hannes.johansson@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Graduate</t>
-        </is>
+          <t>Master's student</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>7</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Information Technology</t>
+          <t xml:space="preserve">virginia.ramos@astrazeneca.com    </t>
         </is>
       </c>
     </row>
@@ -684,22 +668,20 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Elisa Lai</t>
+          <t>Mona Tilly</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>yonglin.lai@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>PhD student</t>
-        </is>
+          <t>Entry-level position (&lt;3 years of experience)</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>8</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>mona.tilly@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -716,44 +698,40 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
+          <t>Master's student</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>9</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
           <t>sophie.you@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Master's student</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Pharmaceutical Science</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Group-3</t>
+          <t>Group-2</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Virginia Ramos</t>
+          <t>Aikaterini Emmanouilidi</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t xml:space="preserve">virginia.ramos@astrazeneca.com    </t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Master's student</t>
-        </is>
+          <t>Mid-level position (3-10 years experience)</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>10</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>DMPK</t>
+          <t>aikaterini.emmanouilidi@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -765,22 +743,20 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Michalis</t>
+          <t>Madeleine Jolliffe</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>michail.fardis@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Mid-level position (3-10 years experience)</t>
-        </is>
+          <t>Graduate</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>11</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Clinical trials</t>
+          <t>maddi.jolliffe@astrazenca.com</t>
         </is>
       </c>
     </row>
@@ -792,22 +768,20 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Aikaterini Emmanouilidi</t>
+          <t>Philip Dalsbecker</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>aikaterini.emmanouilidi@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Mid-level position (3-10 years experience)</t>
-        </is>
+          <t>Post doc</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>12</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Clinical trials</t>
+          <t>philip.dalsbecker@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -819,22 +793,20 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Mona Tilly</t>
+          <t>Elena</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>mona.tilly@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
           <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
+      <c r="D15" t="n">
+        <v>13</v>
+      </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>eleni.lazaridi@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -846,49 +818,45 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Pernilla Rumin</t>
+          <t>Evgeniia Berishvili</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>pernilla.rumin@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
           <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
+      <c r="D16" t="n">
+        <v>14</v>
+      </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Clinical trials</t>
+          <t>evgeniia.berishvili@astrazeneca.com</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Group-4</t>
+          <t>Group-3</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Madeleine Jolliffe</t>
+          <t>Pernilla Rumin</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>maddi.jolliffe@astrazenca.com</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Graduate</t>
-        </is>
+          <t>Mid-level position (3-10 years experience)</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>15</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>pernilla.rumin@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -900,22 +868,20 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Evgeniia Berishvili</t>
+          <t>Michalis</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>evgeniia.berishvili@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
           <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
+      <c r="D18" t="n">
+        <v>16</v>
+      </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Regulatory</t>
+          <t>michail.fardis@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -927,22 +893,20 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Philip Dalsbecker</t>
+          <t>Susanne Sauer</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>philip.dalsbecker@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Post doc</t>
-        </is>
+          <t>Entry-level position (&lt;3 years of experience)</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>17</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>susanne.sauer@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -954,22 +918,20 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Camille Riff</t>
+          <t>Ingrid Lichtin</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Camille.riff@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
           <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
+      <c r="D20" t="n">
+        <v>18</v>
+      </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t xml:space="preserve">CPQP </t>
+          <t>Ingrid.Lichtin@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -981,49 +943,45 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Elena</t>
+          <t>Fatima Eken</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>eleni.lazaridi@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
           <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
+      <c r="D21" t="n">
+        <v>19</v>
+      </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>Kdht135@astrazeneca.com</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Group-5</t>
+          <t>Group-4</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Susanne Sauer</t>
+          <t>Camille Riff</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>susanne.sauer@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
-        </is>
+          <t>Mid-level position (3-10 years experience)</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>20</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>Camille.riff@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1035,22 +993,20 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Arthur Herren</t>
+          <t>Barbara Adamczyk</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Arthur.herren@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>Master's student</t>
-        </is>
+          <t>Senior position (&gt;10 years experience)</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>21</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>barbara.adamczyk@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1062,22 +1018,20 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Ingrid Lichtin</t>
+          <t>Özge Yoluk</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Ingrid.Lichtin@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
           <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
+      <c r="D24" t="n">
+        <v>22</v>
+      </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Quality</t>
+          <t>ozge.yoluk@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1089,22 +1043,20 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Fatima Eken</t>
+          <t>Arthur Herren</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Kdht135@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
-        </is>
+          <t>Master's student</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>23</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>Arthur.herren@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1116,49 +1068,45 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Andrea Elser</t>
+          <t>Megan Lee</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>andrea.elser@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>Post doc</t>
-        </is>
+          <t>Mid-level position (3-10 years experience)</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>24</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>megan.lee2@astrazeneca.com</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Group-6</t>
+          <t>Group-5</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Barbara Adamczyk</t>
+          <t>Maher abduljabbar</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>barbara.adamczyk@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>Senior position (&gt;10 years experience)</t>
-        </is>
+          <t>Entry-level position (&lt;3 years of experience)</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>25</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>maher.abduljabbaral-barooki@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1170,22 +1118,20 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Salma Nahra</t>
+          <t>Andrea Elser</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>salma.nahra1@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>Mid-level position (3-10 years experience)</t>
-        </is>
+          <t>Post doc</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>26</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>andrea.elser@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1197,22 +1143,20 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Anna von Sydow</t>
+          <t>Salma Nahra</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>anna.vonsydow@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>Graduate</t>
-        </is>
+          <t>Mid-level position (3-10 years experience)</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>27</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Data and AI</t>
+          <t>salma.nahra1@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1224,22 +1168,20 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Hemapriya Kothuru Chinnadurai</t>
+          <t>Elena Camara</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>hemapriyakothuru.chinnadurai@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>Master's student</t>
-        </is>
+          <t>Senior position (&gt;10 years experience)</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>28</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>elena.camara@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1251,76 +1193,70 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Megan Lee</t>
+          <t>Anna von Sydow</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>megan.lee2@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>Mid-level position (3-10 years experience)</t>
-        </is>
+          <t>Graduate</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>29</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Innovation</t>
+          <t>anna.vonsydow@astrazeneca.com</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Group-7</t>
+          <t>Group-6</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Özge Yoluk</t>
+          <t>Hemapriya Kothuru Chinnadurai</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>ozge.yoluk@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>Mid-level position (3-10 years experience)</t>
-        </is>
+          <t>Master's student</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>30</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>hemapriyakothuru.chinnadurai@astrazeneca.com</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Group-7</t>
+          <t>Group-6</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Maitreyee Bhalme</t>
+          <t>Christina Chau</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>maitreyee.bhalme@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>Master's student</t>
-        </is>
+          <t>Entry-level position (&lt;3 years of experience)</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>87</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>christina.chau@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1332,22 +1268,20 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Yogesh Aher</t>
+          <t>Ida Näslund</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>yogesh.aher@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
-        </is>
+          <t>Master's student</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>31</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Science generic</t>
+          <t>ida.naslund1@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1359,22 +1293,20 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Maher abduljabbar</t>
+          <t>Víctor López Juan</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>maher.abduljabbaral-barooki@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
           <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
+      <c r="D35" t="n">
+        <v>32</v>
+      </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>victor.lopezjuan@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1386,76 +1318,70 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Emma Källstig</t>
+          <t>Yogesh Aher</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>emma.kallstig@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
           <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
+      <c r="D36" t="n">
+        <v>33</v>
+      </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>yogesh.aher@astrazeneca.com</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Group-8</t>
+          <t>Group-7</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Ida Näslund</t>
+          <t>Maitreyee Bhalme</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>ida.naslund1@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
           <t>Master's student</t>
         </is>
       </c>
+      <c r="D37" t="n">
+        <v>34</v>
+      </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Data and AI</t>
+          <t>maitreyee.bhalme@astrazeneca.com</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Group-8</t>
+          <t>Group-7</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Elena Camara</t>
+          <t>Yuan Wei</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>elena.camara@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>Senior position (&gt;10 years experience)</t>
-        </is>
+          <t>Master's student</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>35</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>yuan.wei7@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1467,22 +1393,20 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Víctor López Juan</t>
+          <t>Emma Källstig</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>victor.lopezjuan@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
           <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
+      <c r="D39" t="n">
+        <v>36</v>
+      </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Clinical trials</t>
+          <t>emma.kallstig@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1494,22 +1418,20 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t xml:space="preserve">Johanna Holm </t>
+          <t>Sushanthika gnanasekaran</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Johanna.holm@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
-        </is>
+          <t>Master's student</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>37</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Quality</t>
+          <t>sushanthika.gnanasekaran@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1521,76 +1443,70 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Yuan Wei</t>
+          <t>Linn Hellberg</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>yuan.wei7@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
           <t>Master's student</t>
         </is>
       </c>
+      <c r="D41" t="n">
+        <v>38</v>
+      </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Data and AI</t>
+          <t>linn.hellberg1@astrazeneca.com</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Group-9</t>
+          <t>Group-8</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Sushanthika gnanasekaran</t>
+          <t>Yannis Asproudis</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>sushanthika.gnanasekaran@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>Master's student</t>
-        </is>
+          <t>Mid-level position (3-10 years experience)</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>39</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Data and AI</t>
+          <t>ioannis.asproudis@astrazeneca.com</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Group-9</t>
+          <t>Group-8</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Yannis Asproudis</t>
+          <t xml:space="preserve">Johanna Holm </t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>ioannis.asproudis@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>Mid-level position (3-10 years experience)</t>
-        </is>
+          <t>Entry-level position (&lt;3 years of experience)</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>40</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>Johanna.holm@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1602,22 +1518,20 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Linn Hellberg</t>
+          <t>Jessica Eriksson</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>linn.hellberg1@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>Master's student</t>
-        </is>
+          <t>Mid-level position (3-10 years experience)</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>41</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Data and AI</t>
+          <t>jessica.eriksson1@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1629,22 +1543,20 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Mia Melhuish</t>
+          <t>Manesh Nautiyal</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>mia.melhuish1@astrazeneca.net</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>Graduate</t>
-        </is>
+          <t>Entry-level position (&lt;3 years of experience)</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>42</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>Manesh.nautiyal@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1656,76 +1568,70 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Manesh Nautiyal</t>
+          <t>Anna</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Manesh.nautiyal@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
-        </is>
+          <t>Post doc</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>43</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>anna.shiriaeva@astrazeneca.com</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Group-10</t>
+          <t>Group-9</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Anna</t>
+          <t>Mia Melhuish</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>anna.shiriaeva@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>Post doc</t>
-        </is>
+          <t>Graduate</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>44</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>mia.melhuish1@astrazeneca.net</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Group-10</t>
+          <t>Group-9</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Adia Groza</t>
+          <t>Maëlys Chastel</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>adia.groza@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>Senior position (&gt;10 years experience)</t>
-        </is>
+          <t>Mid-level position (3-10 years experience)</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>45</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Quality</t>
+          <t>maelys.chastel@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1737,22 +1643,20 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Jessica Eriksson</t>
+          <t>Adia Groza</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>jessica.eriksson1@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>Mid-level position (3-10 years experience)</t>
-        </is>
+          <t>Senior position (&gt;10 years experience)</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>46</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>adia.groza@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1764,22 +1668,20 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Maëlys Chastel</t>
+          <t>Johan Almlöf Ljungberg</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>maelys.chastel@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>Mid-level position (3-10 years experience)</t>
-        </is>
+          <t>Graduate</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>47</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>DS AssayDev</t>
+          <t>johan.almlofljungberg1@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1791,76 +1693,70 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Johan Almlöf Ljungberg</t>
+          <t>Naixuan Liao</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>johan.almlofljungberg1@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>Graduate</t>
-        </is>
+          <t>Entry-level position (&lt;3 years of experience)</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>48</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>naixuan.liao@astrazeneca.com</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Group-11</t>
+          <t>Group-10</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Naixuan Liao</t>
+          <t>Julia Lebrethon</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>naixuan.liao@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
-        </is>
+          <t>Master's student</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>49</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>julia.lebrethon@astrazeneca.com</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Group-11</t>
+          <t>Group-10</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Julia Lebrethon</t>
+          <t>Lara Hastenreiter</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>julia.lebrethon@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>Master's student</t>
-        </is>
+          <t>Contractor</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>50</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>lara.hastenreiter@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1872,22 +1768,20 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Alma söderström</t>
+          <t>Julia Ringwall</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Alma.soderstrom@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>Mid-level position (3-10 years experience)</t>
-        </is>
+          <t>Senior position (&gt;10 years experience)</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>51</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Clinical trials</t>
+          <t>julia.ringwall@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1899,22 +1793,20 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Lara Hastenreiter</t>
+          <t>Alma söderström</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>lara.hastenreiter@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>Contractor</t>
-        </is>
+          <t>Mid-level position (3-10 years experience)</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>52</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>Alma.soderstrom@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1926,76 +1818,70 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Elena Grobecker</t>
+          <t>Aditya Soni</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>elena.grobecker@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>PhD student</t>
-        </is>
+          <t>Entry-level position (&lt;3 years of experience)</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>53</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>aditya.soni@astrazeneca.com</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Group-12</t>
+          <t>Group-11</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Julia Ringwall</t>
+          <t>Elena Grobecker</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>julia.ringwall@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>Senior position (&gt;10 years experience)</t>
-        </is>
+          <t>PhD student</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>54</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t xml:space="preserve">Safety and Work environment </t>
+          <t>elena.grobecker@astrazeneca.com</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Group-12</t>
+          <t>Group-11</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Aditya Soni</t>
+          <t>Charlotte Galipaud</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>aditya.soni@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
           <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
+      <c r="D58" t="n">
+        <v>55</v>
+      </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Discovery Sciences</t>
+          <t>charlotte.galipaud@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -2007,22 +1893,20 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Cristina Secianski</t>
+          <t>Amir Tohidi</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>cristina.secianski@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
           <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
+      <c r="D59" t="n">
+        <v>56</v>
+      </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Regulatory</t>
+          <t>amir.tohidi@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -2034,22 +1918,20 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Charlotte Galipaud</t>
+          <t>Cristina Secianski</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>charlotte.galipaud@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
-        </is>
+          <t>Mid-level position (3-10 years experience)</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>57</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>cristina.secianski@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -2061,76 +1943,70 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Lars Löfgren</t>
+          <t>Giulia Botta</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Lars.lofgren@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>Senior position (&gt;10 years experience)</t>
-        </is>
+          <t>Graduate</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>58</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Translational Science &amp; Experimental Medicine</t>
+          <t>giulia.botta@astrazeneca.com</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Group-13</t>
+          <t>Group-12</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Amir Tohidi</t>
+          <t>Lars Löfgren</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>amir.tohidi@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>Mid-level position (3-10 years experience)</t>
-        </is>
+          <t>Senior position (&gt;10 years experience)</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>59</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Information Technology</t>
+          <t>Lars.lofgren@astrazeneca.com</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Group-13</t>
+          <t>Group-12</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Alisa Kirkin</t>
+          <t>Umul-Khair Noor</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>alisa.kirkin@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>Master's student</t>
-        </is>
+          <t>Mid-level position (3-10 years experience)</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>60</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>umul-khair.noor@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -2142,22 +2018,20 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Purusothaman Seenivasan</t>
+          <t>Danielle Paterson</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>purusothaman.seenivasan@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>Master's student</t>
-        </is>
+          <t>Entry-level position (&lt;3 years of experience)</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>61</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Data and AI</t>
+          <t>danielle.paterson@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -2169,22 +2043,20 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Umul-Khair Noor</t>
+          <t>Holly Longhurst</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>umul-khair.noor@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>Mid-level position (3-10 years experience)</t>
-        </is>
+          <t>Entry-level position (&lt;3 years of experience)</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>62</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Regulatory</t>
+          <t>holly.longhurst@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -2196,76 +2068,70 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Nina Koo</t>
+          <t>Purusothaman Seenivasan</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>hyewonnina.koo@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>Mid-level position (3-10 years experience)</t>
-        </is>
+          <t>Master's student</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>63</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Data and AI</t>
+          <t>purusothaman.seenivasan@astrazeneca.com</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Group-14</t>
+          <t>Group-13</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Saja Hasan</t>
+          <t>Susanna Abrahmsen Alami</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>saja.hasan@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
-        </is>
+          <t>Senior position (&gt;10 years experience)</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>64</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Quality</t>
+          <t>Susanna.Abrahmsen-alami@astrazeneca.com</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Group-14</t>
+          <t>Group-13</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Giulia Botta</t>
+          <t>Miriam Cipullo</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>giulia.botta@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>Graduate</t>
-        </is>
+          <t>Post doc</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>65</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>miriam.cipullo@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -2277,22 +2143,20 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Melanie Hendrix</t>
+          <t>Alisa Kirkin</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>melanie.hendrix@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>Mid-level position (3-10 years experience)</t>
-        </is>
+          <t>Master's student</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>66</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Regulatory</t>
+          <t>alisa.kirkin@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -2304,22 +2168,20 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Danielle Paterson</t>
+          <t>Nina Koo</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>danielle.paterson@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
-        </is>
+          <t>Mid-level position (3-10 years experience)</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>67</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>hyewonnina.koo@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -2331,76 +2193,70 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Bhavik Chouhan</t>
+          <t>Saja Hasan</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>bhavik.chouhan@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>Mid-level position (3-10 years experience)</t>
-        </is>
+          <t>Entry-level position (&lt;3 years of experience)</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>68</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Data and AI</t>
+          <t>saja.hasan@astrazeneca.com</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Group-15</t>
+          <t>Group-14</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Holly Longhurst</t>
+          <t>Melanie Hendrix</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>holly.longhurst@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
-        </is>
+          <t>Mid-level position (3-10 years experience)</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>69</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>melanie.hendrix@astrazeneca.com</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Group-15</t>
+          <t>Group-14</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Susanna Abrahmsen Alami</t>
+          <t>Charline Sommer</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Susanna.Abrahmsen-alami@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>Senior position (&gt;10 years experience)</t>
-        </is>
+          <t>Post doc</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>70</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>Charline.sommer@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -2412,22 +2268,20 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Kim Stockfelt</t>
+          <t>Bhavik Chouhan</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Kim.stockfelt@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr">
-        <is>
           <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
+      <c r="D74" t="n">
+        <v>71</v>
+      </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>bhavik.chouhan@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -2439,22 +2293,20 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Miriam Cipullo</t>
+          <t>Lakshidaa</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>miriam.cipullo@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>Post doc</t>
-        </is>
+          <t>Mid-level position (3-10 years experience)</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>72</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>lakshidaa.saigiridharan@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -2466,29 +2318,27 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Manu Kanti</t>
+          <t>Kim Stockfelt</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>manumanjunath.kanti@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
-        </is>
+          <t>Mid-level position (3-10 years experience)</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>73</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>Kim.stockfelt@astrazeneca.com</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Group-16</t>
+          <t>Group-15</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2498,44 +2348,40 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
+          <t>Mid-level position (3-10 years experience)</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>74</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
           <t>Yinan.song@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>Mid-level position (3-10 years experience)</t>
-        </is>
-      </c>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>Chemistry</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Group-16</t>
+          <t>Group-15</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Lakshidaa</t>
+          <t>Tho Nguyen</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>lakshidaa.saigiridharan@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr">
-        <is>
           <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
+      <c r="D78" t="n">
+        <v>75</v>
+      </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Data and AI</t>
+          <t>tho.nguyen1@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -2547,22 +2393,20 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Alina Khramova</t>
+          <t xml:space="preserve">Elin Benatti </t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Alina.khramova@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>Mid-level position (3-10 years experience)</t>
-        </is>
+          <t>Entry-level position (&lt;3 years of experience)</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>76</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Management</t>
+          <t>elin.benatti1@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -2574,22 +2418,20 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Charline Sommer</t>
+          <t>Manu Kanti</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Charline.sommer@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>Post doc</t>
-        </is>
+          <t>Entry-level position (&lt;3 years of experience)</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>77</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>manumanjunath.kanti@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -2601,76 +2443,70 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t xml:space="preserve">Elin Benatti </t>
+          <t>Alison Howett</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>elin.benatti1@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
           <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
+      <c r="D81" t="n">
+        <v>78</v>
+      </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>alison.howett@astrazeneca.com</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Group-17</t>
+          <t>Group-16</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Tho Nguyen</t>
+          <t>Pavlos Kashioulis</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>tho.nguyen1@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D82" t="inlineStr">
-        <is>
           <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
+      <c r="D82" t="n">
+        <v>79</v>
+      </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Pharmaceutical Science</t>
+          <t>pavlos.kashioulis@astrazeneca.com</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Group-17</t>
+          <t>Group-16</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Pavlos Kashioulis</t>
+          <t>Alina Khramova</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>pavlos.kashioulis@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D83" t="inlineStr">
-        <is>
           <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
+      <c r="D83" t="n">
+        <v>80</v>
+      </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Clinical trials</t>
+          <t>Alina.khramova@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -2682,22 +2518,20 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Alison Howett</t>
+          <t xml:space="preserve">Jennifer Sjulander </t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>alison.howett@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D84" t="inlineStr">
-        <is>
           <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
+      <c r="D84" t="n">
+        <v>81</v>
+      </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Regulatory</t>
+          <t>Jennifer.sjulander2@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -2714,17 +2548,15 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
+          <t>Post doc</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>82</v>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
           <t>michael.guerzoni@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>Post doc</t>
-        </is>
-      </c>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>Chemistry</t>
         </is>
       </c>
     </row>
@@ -2736,29 +2568,27 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t xml:space="preserve">Jennifer Sjulander </t>
+          <t xml:space="preserve">Yousra Yahia </t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Jennifer.sjulander2@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
-        </is>
+          <t>Mid-level position (3-10 years experience)</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>83</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Sustainability in R&amp;D</t>
+          <t>Yousra.yahia@astrazeneca.com</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Group-18</t>
+          <t>Group-17</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -2768,44 +2598,40 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
+          <t>Entry-level position (&lt;3 years of experience)</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>84</v>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
           <t>nina.sandstrom@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
-        </is>
-      </c>
-      <c r="E87" t="inlineStr">
-        <is>
-          <t>FM</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Group-18</t>
+          <t>Group-17</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t xml:space="preserve">Yousra Yahia </t>
+          <t>Gabriel Abreu</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Yousra.yahia@astrazeneca.com</t>
-        </is>
-      </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>Mid-level position (3-10 years experience)</t>
-        </is>
+          <t>Senior position (&gt;10 years experience)</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>85</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Bioscience</t>
+          <t>gabriel.abreu@astrazeneca.com</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
facelift. stratified split and then greedy assignemnt
</commit_message>
<xml_diff>
--- a/group_assignments.xlsx
+++ b/group_assignments.xlsx
@@ -476,8 +476,10 @@
           <t>Master's student</t>
         </is>
       </c>
-      <c r="D2" t="n">
-        <v>1</v>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Clinical trials</t>
+        </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -501,8 +503,10 @@
           <t>Graduate</t>
         </is>
       </c>
-      <c r="D3" t="n">
-        <v>2</v>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Information Technology</t>
+        </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -526,8 +530,10 @@
           <t>PhD student</t>
         </is>
       </c>
-      <c r="D4" t="n">
-        <v>3</v>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Data and AI</t>
+        </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -551,8 +557,10 @@
           <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
-      <c r="D5" t="n">
-        <v>4</v>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Pharmaceutical Science</t>
+        </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -576,8 +584,10 @@
           <t>PhD student</t>
         </is>
       </c>
-      <c r="D6" t="n">
-        <v>5</v>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Chemistry</t>
+        </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -588,25 +598,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Group-1</t>
+          <t>Group-2</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Ulrike Ulbricht</t>
+          <t>Fabricio Belgrano</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Senior position (&gt;10 years experience)</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>86</v>
+          <t>Entry-level position (&lt;3 years of experience)</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Intellectual Property</t>
+        </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Ulrike.ulbricht@astrazeneca.com</t>
+          <t>fabricio.belgrano@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -618,20 +630,22 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Fabricio Belgrano</t>
+          <t>Virginia Ramos</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>6</v>
+          <t>Master's student</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>DMPK</t>
+        </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>fabricio.belgrano@astrazeneca.com</t>
+          <t xml:space="preserve">virginia.ramos@astrazeneca.com    </t>
         </is>
       </c>
     </row>
@@ -643,20 +657,22 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Virginia Ramos</t>
+          <t>Mona Tilly</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Master's student</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>7</v>
+          <t>Entry-level position (&lt;3 years of experience)</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Pharmaceutical Science</t>
+        </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t xml:space="preserve">virginia.ramos@astrazeneca.com    </t>
+          <t>mona.tilly@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -668,20 +684,22 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Mona Tilly</t>
+          <t>Sophie You</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>8</v>
+          <t>Master's student</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Pharmaceutical Science</t>
+        </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>mona.tilly@astrazeneca.com</t>
+          <t>sophie.you@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -693,45 +711,49 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Sophie You</t>
+          <t>Aikaterini Emmanouilidi</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Master's student</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>9</v>
+          <t>Mid-level position (3-10 years experience)</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Clinical trials</t>
+        </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>sophie.you@astrazeneca.com</t>
+          <t>aikaterini.emmanouilidi@astrazeneca.com</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Group-2</t>
+          <t>Group-3</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Aikaterini Emmanouilidi</t>
+          <t>Madeleine Jolliffe</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>10</v>
+          <t>Graduate</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Bioscience</t>
+        </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>aikaterini.emmanouilidi@astrazeneca.com</t>
+          <t>maddi.jolliffe@astrazenca.com</t>
         </is>
       </c>
     </row>
@@ -743,20 +765,22 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Madeleine Jolliffe</t>
+          <t>Philip Dalsbecker</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Graduate</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>11</v>
+          <t>Post doc</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Bioscience</t>
+        </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>maddi.jolliffe@astrazenca.com</t>
+          <t>philip.dalsbecker@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -768,20 +792,22 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Philip Dalsbecker</t>
+          <t>Elena</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Post doc</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>12</v>
+          <t>Entry-level position (&lt;3 years of experience)</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Chemistry</t>
+        </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>philip.dalsbecker@astrazeneca.com</t>
+          <t>eleni.lazaridi@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -793,20 +819,22 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Elena</t>
+          <t>Evgeniia Berishvili</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>13</v>
+          <t>Mid-level position (3-10 years experience)</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Regulatory</t>
+        </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>eleni.lazaridi@astrazeneca.com</t>
+          <t>evgeniia.berishvili@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -818,7 +846,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Evgeniia Berishvili</t>
+          <t>Pernilla Rumin</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -826,24 +854,26 @@
           <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
-      <c r="D16" t="n">
-        <v>14</v>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Clinical trials</t>
+        </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>evgeniia.berishvili@astrazeneca.com</t>
+          <t>pernilla.rumin@astrazeneca.com</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Group-3</t>
+          <t>Group-4</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Pernilla Rumin</t>
+          <t>Michalis</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -851,12 +881,14 @@
           <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
-      <c r="D17" t="n">
-        <v>15</v>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Clinical trials</t>
+        </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>pernilla.rumin@astrazeneca.com</t>
+          <t>michail.fardis@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -868,20 +900,22 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Michalis</t>
+          <t>Susanne Sauer</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
-        <v>16</v>
+          <t>Entry-level position (&lt;3 years of experience)</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Chemistry</t>
+        </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>michail.fardis@astrazeneca.com</t>
+          <t>susanne.sauer@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -893,20 +927,22 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Susanne Sauer</t>
+          <t>Ingrid Lichtin</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>17</v>
+          <t>Mid-level position (3-10 years experience)</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Quality</t>
+        </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>susanne.sauer@astrazeneca.com</t>
+          <t>Ingrid.Lichtin@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -918,20 +954,22 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Ingrid Lichtin</t>
+          <t>Fatima Eken</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>18</v>
+          <t>Entry-level position (&lt;3 years of experience)</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Pharmaceutical Science</t>
+        </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Ingrid.Lichtin@astrazeneca.com</t>
+          <t>Kdht135@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -943,45 +981,49 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Fatima Eken</t>
+          <t>Camille Riff</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
-        <v>19</v>
+          <t>Mid-level position (3-10 years experience)</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CPQP </t>
+        </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Kdht135@astrazeneca.com</t>
+          <t>Camille.riff@astrazeneca.com</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Group-4</t>
+          <t>Group-5</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Camille Riff</t>
+          <t>Barbara Adamczyk</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
-        <v>20</v>
+          <t>Senior position (&gt;10 years experience)</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Pharmaceutical Science</t>
+        </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Camille.riff@astrazeneca.com</t>
+          <t>barbara.adamczyk@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -993,20 +1035,22 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Barbara Adamczyk</t>
+          <t>Özge Yoluk</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Senior position (&gt;10 years experience)</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
-        <v>21</v>
+          <t>Mid-level position (3-10 years experience)</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Chemistry</t>
+        </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>barbara.adamczyk@astrazeneca.com</t>
+          <t>ozge.yoluk@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1018,20 +1062,22 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Özge Yoluk</t>
+          <t>Arthur Herren</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
-        </is>
-      </c>
-      <c r="D24" t="n">
-        <v>22</v>
+          <t>Master's student</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Pharmaceutical Science</t>
+        </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>ozge.yoluk@astrazeneca.com</t>
+          <t>Arthur.herren@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1043,20 +1089,22 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Arthur Herren</t>
+          <t>Megan Lee</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Master's student</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
-        <v>23</v>
+          <t>Mid-level position (3-10 years experience)</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Innovation</t>
+        </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Arthur.herren@astrazeneca.com</t>
+          <t>megan.lee2@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1068,45 +1116,49 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Megan Lee</t>
+          <t>Maher abduljabbar</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
-        </is>
-      </c>
-      <c r="D26" t="n">
-        <v>24</v>
+          <t>Entry-level position (&lt;3 years of experience)</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Pharmaceutical Science</t>
+        </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>megan.lee2@astrazeneca.com</t>
+          <t>maher.abduljabbaral-barooki@astrazeneca.com</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Group-5</t>
+          <t>Group-6</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Maher abduljabbar</t>
+          <t>Andrea Elser</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
-        </is>
-      </c>
-      <c r="D27" t="n">
-        <v>25</v>
+          <t>Post doc</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Bioscience</t>
+        </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>maher.abduljabbaral-barooki@astrazeneca.com</t>
+          <t>andrea.elser@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1118,20 +1170,22 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Andrea Elser</t>
+          <t>Salma Nahra</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Post doc</t>
-        </is>
-      </c>
-      <c r="D28" t="n">
-        <v>26</v>
+          <t>Mid-level position (3-10 years experience)</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Pharmaceutical Science</t>
+        </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>andrea.elser@astrazeneca.com</t>
+          <t>salma.nahra1@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1143,20 +1197,22 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Salma Nahra</t>
+          <t>Elena Camara</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
-        </is>
-      </c>
-      <c r="D29" t="n">
-        <v>27</v>
+          <t>Senior position (&gt;10 years experience)</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Bioscience</t>
+        </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>salma.nahra1@astrazeneca.com</t>
+          <t>elena.camara@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1168,20 +1224,22 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Elena Camara</t>
+          <t>Anna von Sydow</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Senior position (&gt;10 years experience)</t>
-        </is>
-      </c>
-      <c r="D30" t="n">
-        <v>28</v>
+          <t>Graduate</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Data and AI</t>
+        </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>elena.camara@astrazeneca.com</t>
+          <t>anna.vonsydow@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1193,32 +1251,34 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Anna von Sydow</t>
+          <t>Hemapriya Kothuru Chinnadurai</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Graduate</t>
-        </is>
-      </c>
-      <c r="D31" t="n">
-        <v>29</v>
+          <t>Master's student</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Bioscience</t>
+        </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>anna.vonsydow@astrazeneca.com</t>
+          <t>hemapriyakothuru.chinnadurai@astrazeneca.com</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Group-6</t>
+          <t>Group-7</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Hemapriya Kothuru Chinnadurai</t>
+          <t>Ida Näslund</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1226,24 +1286,26 @@
           <t>Master's student</t>
         </is>
       </c>
-      <c r="D32" t="n">
-        <v>30</v>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Data and AI</t>
+        </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>hemapriyakothuru.chinnadurai@astrazeneca.com</t>
+          <t>ida.naslund1@astrazeneca.com</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Group-6</t>
+          <t>Group-7</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Christina Chau</t>
+          <t>Víctor López Juan</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1251,12 +1313,14 @@
           <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
-      <c r="D33" t="n">
-        <v>87</v>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Clinical trials</t>
+        </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>christina.chau@astrazeneca.com</t>
+          <t>victor.lopezjuan@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1268,20 +1332,22 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Ida Näslund</t>
+          <t>Yogesh Aher</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Master's student</t>
-        </is>
-      </c>
-      <c r="D34" t="n">
-        <v>31</v>
+          <t>Entry-level position (&lt;3 years of experience)</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Science generic</t>
+        </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>ida.naslund1@astrazeneca.com</t>
+          <t>yogesh.aher@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1293,20 +1359,22 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Víctor López Juan</t>
+          <t>Maitreyee Bhalme</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
-        </is>
-      </c>
-      <c r="D35" t="n">
-        <v>32</v>
+          <t>Master's student</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Bioscience</t>
+        </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>victor.lopezjuan@astrazeneca.com</t>
+          <t>maitreyee.bhalme@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1318,57 +1386,61 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Yogesh Aher</t>
+          <t>Yuan Wei</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
-        </is>
-      </c>
-      <c r="D36" t="n">
-        <v>33</v>
+          <t>Master's student</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Data and AI</t>
+        </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>yogesh.aher@astrazeneca.com</t>
+          <t>yuan.wei7@astrazeneca.com</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Group-7</t>
+          <t>Group-8</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Maitreyee Bhalme</t>
+          <t>Emma Källstig</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Master's student</t>
-        </is>
-      </c>
-      <c r="D37" t="n">
-        <v>34</v>
+          <t>Entry-level position (&lt;3 years of experience)</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Bioscience</t>
+        </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>maitreyee.bhalme@astrazeneca.com</t>
+          <t>emma.kallstig@astrazeneca.com</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Group-7</t>
+          <t>Group-8</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Yuan Wei</t>
+          <t>Sushanthika gnanasekaran</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1376,12 +1448,14 @@
           <t>Master's student</t>
         </is>
       </c>
-      <c r="D38" t="n">
-        <v>35</v>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Data and AI</t>
+        </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>yuan.wei7@astrazeneca.com</t>
+          <t>sushanthika.gnanasekaran@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1393,20 +1467,22 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Emma Källstig</t>
+          <t>Linn Hellberg</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
-        </is>
-      </c>
-      <c r="D39" t="n">
-        <v>36</v>
+          <t>Master's student</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Data and AI</t>
+        </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>emma.kallstig@astrazeneca.com</t>
+          <t>linn.hellberg1@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1418,20 +1494,22 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Sushanthika gnanasekaran</t>
+          <t>Yannis Asproudis</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Master's student</t>
-        </is>
-      </c>
-      <c r="D40" t="n">
-        <v>37</v>
+          <t>Mid-level position (3-10 years experience)</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Pharmaceutical Science</t>
+        </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>sushanthika.gnanasekaran@astrazeneca.com</t>
+          <t>ioannis.asproudis@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1443,20 +1521,22 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Linn Hellberg</t>
+          <t xml:space="preserve">Johanna Holm </t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Master's student</t>
-        </is>
-      </c>
-      <c r="D41" t="n">
-        <v>38</v>
+          <t>Entry-level position (&lt;3 years of experience)</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Quality</t>
+        </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>linn.hellberg1@astrazeneca.com</t>
+          <t>Johanna.holm@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1468,45 +1548,49 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Yannis Asproudis</t>
+          <t>Ulrike Ulbricht</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
-        </is>
-      </c>
-      <c r="D42" t="n">
-        <v>39</v>
+          <t>Senior position (&gt;10 years experience)</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Clinical trials</t>
+        </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>ioannis.asproudis@astrazeneca.com</t>
+          <t>Ulrike.ulbricht@astrazeneca.com</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Group-8</t>
+          <t>Group-9</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t xml:space="preserve">Johanna Holm </t>
+          <t>Jessica Eriksson</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
-        </is>
-      </c>
-      <c r="D43" t="n">
-        <v>40</v>
+          <t>Mid-level position (3-10 years experience)</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Pharmaceutical Science</t>
+        </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Johanna.holm@astrazeneca.com</t>
+          <t>jessica.eriksson1@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1518,20 +1602,22 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Jessica Eriksson</t>
+          <t>Manesh Nautiyal</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
-        </is>
-      </c>
-      <c r="D44" t="n">
-        <v>41</v>
+          <t>Entry-level position (&lt;3 years of experience)</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Chemistry</t>
+        </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>jessica.eriksson1@astrazeneca.com</t>
+          <t>Manesh.nautiyal@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1543,20 +1629,22 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Manesh Nautiyal</t>
+          <t>Anna</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
-        </is>
-      </c>
-      <c r="D45" t="n">
-        <v>42</v>
+          <t>Post doc</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Bioscience</t>
+        </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Manesh.nautiyal@astrazeneca.com</t>
+          <t>anna.shiriaeva@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1568,20 +1656,22 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Anna</t>
+          <t>Mia Melhuish</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Post doc</t>
-        </is>
-      </c>
-      <c r="D46" t="n">
-        <v>43</v>
+          <t>Graduate</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Bioscience</t>
+        </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>anna.shiriaeva@astrazeneca.com</t>
+          <t>mia.melhuish1@astrazeneca.net</t>
         </is>
       </c>
     </row>
@@ -1593,45 +1683,49 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Mia Melhuish</t>
+          <t>Maëlys Chastel</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Graduate</t>
-        </is>
-      </c>
-      <c r="D47" t="n">
-        <v>44</v>
+          <t>Mid-level position (3-10 years experience)</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>DS AssayDev</t>
+        </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>mia.melhuish1@astrazeneca.net</t>
+          <t>maelys.chastel@astrazeneca.com</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Group-9</t>
+          <t>Group-10</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Maëlys Chastel</t>
+          <t>Adia Groza</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
-        </is>
-      </c>
-      <c r="D48" t="n">
-        <v>45</v>
+          <t>Senior position (&gt;10 years experience)</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Quality</t>
+        </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>maelys.chastel@astrazeneca.com</t>
+          <t>adia.groza@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1643,20 +1737,22 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Adia Groza</t>
+          <t>Johan Almlöf Ljungberg</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Senior position (&gt;10 years experience)</t>
-        </is>
-      </c>
-      <c r="D49" t="n">
-        <v>46</v>
+          <t>Graduate</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Pharmaceutical Science</t>
+        </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>adia.groza@astrazeneca.com</t>
+          <t>johan.almlofljungberg1@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1668,20 +1764,22 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Johan Almlöf Ljungberg</t>
+          <t>Naixuan Liao</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Graduate</t>
-        </is>
-      </c>
-      <c r="D50" t="n">
-        <v>47</v>
+          <t>Entry-level position (&lt;3 years of experience)</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Bioscience</t>
+        </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>johan.almlofljungberg1@astrazeneca.com</t>
+          <t>naixuan.liao@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1693,20 +1791,22 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Naixuan Liao</t>
+          <t>Julia Lebrethon</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
-        </is>
-      </c>
-      <c r="D51" t="n">
-        <v>48</v>
+          <t>Master's student</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Pharmaceutical Science</t>
+        </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>naixuan.liao@astrazeneca.com</t>
+          <t>julia.lebrethon@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1718,45 +1818,49 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Julia Lebrethon</t>
+          <t>Lara Hastenreiter</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Master's student</t>
-        </is>
-      </c>
-      <c r="D52" t="n">
-        <v>49</v>
+          <t>Contractor</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Maintenance</t>
+        </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>julia.lebrethon@astrazeneca.com</t>
+          <t>lara.hastenreiter@astrazeneca.com</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Group-10</t>
+          <t>Group-11</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Lara Hastenreiter</t>
+          <t>Julia Ringwall</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Contractor</t>
-        </is>
-      </c>
-      <c r="D53" t="n">
-        <v>50</v>
+          <t>Senior position (&gt;10 years experience)</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Safety and Work environment </t>
+        </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>lara.hastenreiter@astrazeneca.com</t>
+          <t>julia.ringwall@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1768,20 +1872,22 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Julia Ringwall</t>
+          <t>Alma söderström</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Senior position (&gt;10 years experience)</t>
-        </is>
-      </c>
-      <c r="D54" t="n">
-        <v>51</v>
+          <t>Mid-level position (3-10 years experience)</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Clinical trials</t>
+        </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>julia.ringwall@astrazeneca.com</t>
+          <t>Alma.soderstrom@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1793,20 +1899,22 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Alma söderström</t>
+          <t>Aditya Soni</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
-        </is>
-      </c>
-      <c r="D55" t="n">
-        <v>52</v>
+          <t>Entry-level position (&lt;3 years of experience)</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Discovery Sciences</t>
+        </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Alma.soderstrom@astrazeneca.com</t>
+          <t>aditya.soni@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1818,20 +1926,22 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Aditya Soni</t>
+          <t>Elena Grobecker</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
-        </is>
-      </c>
-      <c r="D56" t="n">
-        <v>53</v>
+          <t>PhD student</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Pharmaceutical Science</t>
+        </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>aditya.soni@astrazeneca.com</t>
+          <t>elena.grobecker@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1843,45 +1953,49 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Elena Grobecker</t>
+          <t>Charlotte Galipaud</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>PhD student</t>
-        </is>
-      </c>
-      <c r="D57" t="n">
-        <v>54</v>
+          <t>Entry-level position (&lt;3 years of experience)</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Bioscience</t>
+        </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>elena.grobecker@astrazeneca.com</t>
+          <t>charlotte.galipaud@astrazeneca.com</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Group-11</t>
+          <t>Group-12</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Charlotte Galipaud</t>
+          <t>Amir Tohidi</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Entry-level position (&lt;3 years of experience)</t>
-        </is>
-      </c>
-      <c r="D58" t="n">
-        <v>55</v>
+          <t>Mid-level position (3-10 years experience)</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Information Technology</t>
+        </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>charlotte.galipaud@astrazeneca.com</t>
+          <t>amir.tohidi@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1893,7 +2007,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Amir Tohidi</t>
+          <t>Cristina Secianski</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1901,12 +2015,14 @@
           <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
-      <c r="D59" t="n">
-        <v>56</v>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Regulatory</t>
+        </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>amir.tohidi@astrazeneca.com</t>
+          <t>cristina.secianski@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1918,20 +2034,22 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Cristina Secianski</t>
+          <t>Giulia Botta</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
-        </is>
-      </c>
-      <c r="D60" t="n">
-        <v>57</v>
+          <t>Graduate</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Chemistry</t>
+        </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>cristina.secianski@astrazeneca.com</t>
+          <t>giulia.botta@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1943,20 +2061,22 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Giulia Botta</t>
+          <t>Lars Löfgren</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Graduate</t>
-        </is>
-      </c>
-      <c r="D61" t="n">
-        <v>58</v>
+          <t>Senior position (&gt;10 years experience)</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Translational Science &amp; Experimental Medicine</t>
+        </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>giulia.botta@astrazeneca.com</t>
+          <t>Lars.lofgren@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1968,20 +2088,22 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Lars Löfgren</t>
+          <t>Umul-Khair Noor</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Senior position (&gt;10 years experience)</t>
-        </is>
-      </c>
-      <c r="D62" t="n">
-        <v>59</v>
+          <t>Mid-level position (3-10 years experience)</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Regulatory</t>
+        </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Lars.lofgren@astrazeneca.com</t>
+          <t>umul-khair.noor@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -1993,20 +2115,22 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Umul-Khair Noor</t>
+          <t>Christina Chau</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Mid-level position (3-10 years experience)</t>
-        </is>
-      </c>
-      <c r="D63" t="n">
-        <v>60</v>
+          <t>Entry-level position (&lt;3 years of experience)</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Pharmaceutical Science</t>
+        </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>umul-khair.noor@astrazeneca.com</t>
+          <t>christina.chau@astrazeneca.com</t>
         </is>
       </c>
     </row>
@@ -2026,8 +2150,10 @@
           <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
-      <c r="D64" t="n">
-        <v>61</v>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Chemistry</t>
+        </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -2051,8 +2177,10 @@
           <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
-      <c r="D65" t="n">
-        <v>62</v>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Pharmaceutical Science</t>
+        </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -2076,8 +2204,10 @@
           <t>Master's student</t>
         </is>
       </c>
-      <c r="D66" t="n">
-        <v>63</v>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Data and AI</t>
+        </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2101,8 +2231,10 @@
           <t>Senior position (&gt;10 years experience)</t>
         </is>
       </c>
-      <c r="D67" t="n">
-        <v>64</v>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Pharmaceutical Science</t>
+        </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2126,8 +2258,10 @@
           <t>Post doc</t>
         </is>
       </c>
-      <c r="D68" t="n">
-        <v>65</v>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Bioscience</t>
+        </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -2151,8 +2285,10 @@
           <t>Master's student</t>
         </is>
       </c>
-      <c r="D69" t="n">
-        <v>66</v>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Bioscience</t>
+        </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -2176,8 +2312,10 @@
           <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
-      <c r="D70" t="n">
-        <v>67</v>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Data and AI</t>
+        </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -2201,8 +2339,10 @@
           <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
-      <c r="D71" t="n">
-        <v>68</v>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Quality</t>
+        </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2226,8 +2366,10 @@
           <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
-      <c r="D72" t="n">
-        <v>69</v>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Regulatory</t>
+        </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2251,8 +2393,10 @@
           <t>Post doc</t>
         </is>
       </c>
-      <c r="D73" t="n">
-        <v>70</v>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Bioscience</t>
+        </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2276,8 +2420,10 @@
           <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
-      <c r="D74" t="n">
-        <v>71</v>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Data and AI</t>
+        </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -2301,8 +2447,10 @@
           <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
-      <c r="D75" t="n">
-        <v>72</v>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Data and AI</t>
+        </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2326,8 +2474,10 @@
           <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
-      <c r="D76" t="n">
-        <v>73</v>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Pharmaceutical Science</t>
+        </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2351,8 +2501,10 @@
           <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
-      <c r="D77" t="n">
-        <v>74</v>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Chemistry</t>
+        </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2376,8 +2528,10 @@
           <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
-      <c r="D78" t="n">
-        <v>75</v>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Pharmaceutical Science</t>
+        </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2401,8 +2555,10 @@
           <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
-      <c r="D79" t="n">
-        <v>76</v>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Bioscience</t>
+        </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2426,8 +2582,10 @@
           <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
-      <c r="D80" t="n">
-        <v>77</v>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Bioscience</t>
+        </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2451,8 +2609,10 @@
           <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
-      <c r="D81" t="n">
-        <v>78</v>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Regulatory</t>
+        </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -2476,8 +2636,10 @@
           <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
-      <c r="D82" t="n">
-        <v>79</v>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Clinical trials</t>
+        </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -2501,8 +2663,10 @@
           <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
-      <c r="D83" t="n">
-        <v>80</v>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Management</t>
+        </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -2526,8 +2690,10 @@
           <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
-      <c r="D84" t="n">
-        <v>81</v>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Sustainability in R&amp;D</t>
+        </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -2551,8 +2717,10 @@
           <t>Post doc</t>
         </is>
       </c>
-      <c r="D85" t="n">
-        <v>82</v>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Chemistry</t>
+        </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2576,8 +2744,10 @@
           <t>Mid-level position (3-10 years experience)</t>
         </is>
       </c>
-      <c r="D86" t="n">
-        <v>83</v>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Bioscience</t>
+        </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2601,8 +2771,10 @@
           <t>Entry-level position (&lt;3 years of experience)</t>
         </is>
       </c>
-      <c r="D87" t="n">
-        <v>84</v>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>FM</t>
+        </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -2626,8 +2798,10 @@
           <t>Senior position (&gt;10 years experience)</t>
         </is>
       </c>
-      <c r="D88" t="n">
-        <v>85</v>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Clinical trials</t>
+        </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>

</xml_diff>